<commit_message>
Updates to SPRbased PSC.xlsx with Summary Page
</commit_message>
<xml_diff>
--- a/src/dashboard/data/harvestPolicy/DataFromIan/Removals.xlsx
+++ b/src/dashboard/data/harvestPolicy/DataFromIan/Removals.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="22995" windowHeight="11820"/>
+    <workbookView xWindow="0" yWindow="8420" windowWidth="23000" windowHeight="20140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" iterate="1" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Sport</t>
   </si>
@@ -38,15 +43,34 @@
   <si>
     <t># Removals in thousands of pounds</t>
   </si>
+  <si>
+    <t>Commercial</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -69,13 +93,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -375,28 +407,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F129"/>
+  <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="D131" sqref="B130:D131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -416,7 +448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>1466</v>
       </c>
@@ -436,7 +468,7 @@
         <v>1888</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>1290</v>
       </c>
@@ -456,7 +488,7 @@
         <v>1889</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>1373</v>
       </c>
@@ -476,7 +508,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>2131</v>
       </c>
@@ -496,7 +528,7 @@
         <v>1891</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>2768</v>
       </c>
@@ -516,7 +548,7 @@
         <v>1892</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>3215</v>
       </c>
@@ -536,7 +568,7 @@
         <v>1893</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>3756</v>
       </c>
@@ -556,7 +588,7 @@
         <v>1894</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>4251</v>
       </c>
@@ -576,7 +608,7 @@
         <v>1895</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>5423</v>
       </c>
@@ -596,7 +628,7 @@
         <v>1896</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>6594</v>
       </c>
@@ -616,7 +648,7 @@
         <v>1897</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>7765</v>
       </c>
@@ -636,7 +668,7 @@
         <v>1898</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>8936</v>
       </c>
@@ -656,7 +688,7 @@
         <v>1899</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>13405</v>
       </c>
@@ -676,7 +708,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>17874</v>
       </c>
@@ -696,7 +728,7 @@
         <v>1901</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>22343</v>
       </c>
@@ -716,7 +748,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>25210</v>
       </c>
@@ -736,7 +768,7 @@
         <v>1903</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>28077</v>
       </c>
@@ -756,7 +788,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>22000</v>
       </c>
@@ -776,7 +808,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>36000</v>
       </c>
@@ -796,7 +828,7 @@
         <v>1906</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>50000</v>
       </c>
@@ -816,7 +848,7 @@
         <v>1907</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>50617</v>
       </c>
@@ -836,7 +868,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>51233</v>
       </c>
@@ -856,7 +888,7 @@
         <v>1909</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>51850</v>
       </c>
@@ -876,7 +908,7 @@
         <v>1910</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>56931</v>
       </c>
@@ -896,7 +928,7 @@
         <v>1911</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>60434</v>
       </c>
@@ -916,7 +948,7 @@
         <v>1912</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>66543</v>
       </c>
@@ -936,7 +968,7 @@
         <v>1913</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>67425</v>
       </c>
@@ -956,7 +988,7 @@
         <v>1914</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>68483</v>
       </c>
@@ -976,7 +1008,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>49756</v>
       </c>
@@ -996,7 +1028,7 @@
         <v>1916</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>48599</v>
       </c>
@@ -1016,7 +1048,7 @@
         <v>1917</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>37685</v>
       </c>
@@ -1036,7 +1068,7 @@
         <v>1918</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>40138</v>
       </c>
@@ -1056,7 +1088,7 @@
         <v>1919</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>46615</v>
       </c>
@@ -1076,7 +1108,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>52461</v>
       </c>
@@ -1096,7 +1128,7 @@
         <v>1921</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>42495</v>
       </c>
@@ -1116,7 +1148,7 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>51324</v>
       </c>
@@ -1136,7 +1168,7 @@
         <v>1923</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>53135</v>
       </c>
@@ -1156,7 +1188,7 @@
         <v>1924</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>50664</v>
       </c>
@@ -1176,7 +1208,7 @@
         <v>1925</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>52468</v>
       </c>
@@ -1196,7 +1228,7 @@
         <v>1926</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42">
         <v>54952</v>
       </c>
@@ -1216,7 +1248,7 @@
         <v>1927</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43">
         <v>54260</v>
       </c>
@@ -1236,7 +1268,7 @@
         <v>1928</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44">
         <v>56925</v>
       </c>
@@ -1256,7 +1288,7 @@
         <v>1929</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45">
         <v>49506</v>
       </c>
@@ -1276,7 +1308,7 @@
         <v>1930</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46">
         <v>44222</v>
       </c>
@@ -1296,7 +1328,7 @@
         <v>1931</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47">
         <v>44488</v>
       </c>
@@ -1316,7 +1348,7 @@
         <v>1932</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48">
         <v>46907</v>
       </c>
@@ -1336,7 +1368,7 @@
         <v>1933</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49">
         <v>44718</v>
       </c>
@@ -1356,7 +1388,7 @@
         <v>1934</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50">
         <v>47343</v>
       </c>
@@ -1376,7 +1408,7 @@
         <v>1935</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51">
         <v>48923</v>
       </c>
@@ -1396,7 +1428,7 @@
         <v>1936</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52">
         <v>49539</v>
       </c>
@@ -1416,7 +1448,7 @@
         <v>1937</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53">
         <v>49553</v>
       </c>
@@ -1436,7 +1468,7 @@
         <v>1938</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="A54">
         <v>50903</v>
       </c>
@@ -1456,7 +1488,7 @@
         <v>1939</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55">
         <v>53381</v>
       </c>
@@ -1476,7 +1508,7 @@
         <v>1940</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="A56">
         <v>52231</v>
       </c>
@@ -1496,7 +1528,7 @@
         <v>1941</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="A57">
         <v>50388</v>
       </c>
@@ -1516,7 +1548,7 @@
         <v>1942</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58">
         <v>53699</v>
       </c>
@@ -1536,7 +1568,7 @@
         <v>1943</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59">
         <v>53435</v>
       </c>
@@ -1556,7 +1588,7 @@
         <v>1944</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60">
         <v>53395</v>
       </c>
@@ -1576,7 +1608,7 @@
         <v>1945</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61">
         <v>60266</v>
       </c>
@@ -1596,7 +1628,7 @@
         <v>1946</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="A62">
         <v>55700</v>
       </c>
@@ -1616,7 +1648,7 @@
         <v>1947</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="A63">
         <v>55564</v>
       </c>
@@ -1636,7 +1668,7 @@
         <v>1948</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="A64">
         <v>55025</v>
       </c>
@@ -1656,7 +1688,7 @@
         <v>1949</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6">
       <c r="A65">
         <v>57234</v>
       </c>
@@ -1676,7 +1708,7 @@
         <v>1950</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6">
       <c r="A66">
         <v>56045</v>
       </c>
@@ -1696,7 +1728,7 @@
         <v>1951</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6">
       <c r="A67">
         <v>62262</v>
       </c>
@@ -1716,7 +1748,7 @@
         <v>1952</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6">
       <c r="A68">
         <v>59837</v>
       </c>
@@ -1736,7 +1768,7 @@
         <v>1953</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6">
       <c r="A69">
         <v>70583</v>
       </c>
@@ -1756,7 +1788,7 @@
         <v>1954</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6">
       <c r="A70">
         <v>57521</v>
       </c>
@@ -1776,7 +1808,7 @@
         <v>1955</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6">
       <c r="A71">
         <v>66588</v>
       </c>
@@ -1796,7 +1828,7 @@
         <v>1956</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6">
       <c r="A72">
         <v>60854</v>
       </c>
@@ -1816,7 +1848,7 @@
         <v>1957</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6">
       <c r="A73">
         <v>64508</v>
       </c>
@@ -1836,7 +1868,7 @@
         <v>1958</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6">
       <c r="A74">
         <v>71204</v>
       </c>
@@ -1856,7 +1888,7 @@
         <v>1959</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6">
       <c r="A75">
         <v>71605</v>
       </c>
@@ -1876,7 +1908,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6">
       <c r="A76">
         <v>69274</v>
       </c>
@@ -1896,7 +1928,7 @@
         <v>1961</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6">
       <c r="A77">
         <v>74862</v>
       </c>
@@ -1916,7 +1948,7 @@
         <v>1962</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6">
       <c r="A78">
         <v>71237</v>
       </c>
@@ -1936,7 +1968,7 @@
         <v>1963</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6">
       <c r="A79">
         <v>59784</v>
       </c>
@@ -1956,7 +1988,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6">
       <c r="A80">
         <v>63176</v>
       </c>
@@ -1976,7 +2008,7 @@
         <v>1965</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6">
       <c r="A81">
         <v>62016</v>
       </c>
@@ -1996,7 +2028,7 @@
         <v>1966</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6">
       <c r="A82">
         <v>55222</v>
       </c>
@@ -2016,7 +2048,7 @@
         <v>1967</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6">
       <c r="A83">
         <v>48594</v>
       </c>
@@ -2036,7 +2068,7 @@
         <v>1968</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6">
       <c r="A84">
         <v>58274</v>
       </c>
@@ -2056,7 +2088,7 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6">
       <c r="A85">
         <v>54838</v>
       </c>
@@ -2076,7 +2108,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6">
       <c r="A86">
         <v>46654</v>
       </c>
@@ -2096,7 +2128,7 @@
         <v>1971</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6">
       <c r="A87">
         <v>42884</v>
       </c>
@@ -2116,7 +2148,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6">
       <c r="A88">
         <v>31740</v>
       </c>
@@ -2136,7 +2168,7 @@
         <v>1973</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6">
       <c r="A89">
         <v>21310</v>
       </c>
@@ -2156,7 +2188,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6">
       <c r="A90">
         <v>27620</v>
       </c>
@@ -2176,7 +2208,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6">
       <c r="A91">
         <v>27540</v>
       </c>
@@ -2196,7 +2228,7 @@
         <v>1976</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6">
       <c r="A92">
         <v>21880</v>
       </c>
@@ -2216,7 +2248,7 @@
         <v>1977</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6">
       <c r="A93">
         <v>22000</v>
       </c>
@@ -2236,7 +2268,7 @@
         <v>1978</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6">
       <c r="A94">
         <v>22540</v>
       </c>
@@ -2256,7 +2288,7 @@
         <v>1979</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6">
       <c r="A95">
         <v>21870</v>
       </c>
@@ -2276,7 +2308,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6">
       <c r="A96">
         <v>25736</v>
       </c>
@@ -2296,7 +2328,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6">
       <c r="A97">
         <v>29007</v>
       </c>
@@ -2316,7 +2348,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6">
       <c r="A98">
         <v>38386</v>
       </c>
@@ -2336,7 +2368,7 @@
         <v>1983</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6">
       <c r="A99">
         <v>44971</v>
       </c>
@@ -2356,7 +2388,7 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6">
       <c r="A100">
         <v>57702</v>
       </c>
@@ -2376,7 +2408,7 @@
         <v>1985</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6">
       <c r="A101">
         <v>72832</v>
       </c>
@@ -2396,7 +2428,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6">
       <c r="A102">
         <v>72196</v>
       </c>
@@ -2416,7 +2448,7 @@
         <v>1987</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6">
       <c r="A103">
         <v>76340</v>
       </c>
@@ -2436,7 +2468,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6">
       <c r="A104">
         <v>68975</v>
       </c>
@@ -2456,7 +2488,7 @@
         <v>1989</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6">
       <c r="A105">
         <v>63621</v>
       </c>
@@ -2476,7 +2508,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6">
       <c r="A106">
         <v>59308</v>
       </c>
@@ -2496,7 +2528,7 @@
         <v>1991</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6">
       <c r="A107">
         <v>61145</v>
       </c>
@@ -2516,7 +2548,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6">
       <c r="A108">
         <v>60087</v>
       </c>
@@ -2536,7 +2568,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6">
       <c r="A109">
         <v>56025</v>
       </c>
@@ -2556,7 +2588,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6">
       <c r="A110">
         <v>44142</v>
       </c>
@@ -2576,7 +2608,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6">
       <c r="A111">
         <v>47697</v>
       </c>
@@ -2596,7 +2628,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6">
       <c r="A112">
         <v>65487</v>
       </c>
@@ -2616,7 +2648,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6">
       <c r="A113">
         <v>70127</v>
       </c>
@@ -2636,7 +2668,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6">
       <c r="A114">
         <v>74705</v>
       </c>
@@ -2656,7 +2688,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6">
       <c r="A115">
         <v>68560</v>
       </c>
@@ -2676,7 +2708,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6">
       <c r="A116">
         <v>70980</v>
       </c>
@@ -2696,7 +2728,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6">
       <c r="A117">
         <v>74957</v>
       </c>
@@ -2716,7 +2748,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6">
       <c r="A118">
         <v>73370</v>
       </c>
@@ -2736,7 +2768,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6">
       <c r="A119">
         <v>73314</v>
       </c>
@@ -2756,7 +2788,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6">
       <c r="A120">
         <v>72111</v>
       </c>
@@ -2776,7 +2808,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6">
       <c r="A121">
         <v>68125</v>
       </c>
@@ -2796,7 +2828,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6">
       <c r="A122">
         <v>63032</v>
       </c>
@@ -2816,7 +2848,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6">
       <c r="A123">
         <v>58706</v>
       </c>
@@ -2836,7 +2868,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6">
       <c r="A124">
         <v>52176</v>
       </c>
@@ -2856,7 +2888,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6">
       <c r="A125">
         <v>49825</v>
       </c>
@@ -2876,7 +2908,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6">
       <c r="A126">
         <v>39615</v>
       </c>
@@ -2896,7 +2928,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6">
       <c r="A127">
         <v>32052</v>
       </c>
@@ -2916,7 +2948,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6">
       <c r="A128">
         <v>29126</v>
       </c>
@@ -2936,7 +2968,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6">
       <c r="A129">
         <v>23739</v>
       </c>
@@ -2956,8 +2988,39 @@
         <v>2014</v>
       </c>
     </row>
+    <row r="130" spans="1:6">
+      <c r="B130" t="s">
+        <v>7</v>
+      </c>
+      <c r="C130" t="s">
+        <v>4</v>
+      </c>
+      <c r="D130" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="B131">
+        <f>A129+B129</f>
+        <v>24977</v>
+      </c>
+      <c r="C131">
+        <f>C129</f>
+        <v>9315</v>
+      </c>
+      <c r="D131">
+        <f>D129</f>
+        <v>7083</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2967,9 +3030,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2979,8 +3047,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Huge amounts of updates to TMA.R
</commit_message>
<xml_diff>
--- a/src/dashboard/data/harvestPolicy/DataFromIan/Removals.xlsx
+++ b/src/dashboard/data/harvestPolicy/DataFromIan/Removals.xlsx
@@ -4,14 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8420" windowWidth="23000" windowHeight="20140"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="50640" windowHeight="15500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" iterate="1" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="q">Sheet1!$H$131</definedName>
+  </definedNames>
+  <calcPr calcId="140001" calcMode="autoNoTable" iterate="1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
   <si>
     <t>Sport</t>
   </si>
@@ -46,12 +49,36 @@
   <si>
     <t>Commercial</t>
   </si>
+  <si>
+    <t>Survey</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>Relative Exploitation Rates</t>
+  </si>
+  <si>
+    <t>Personal</t>
+  </si>
+  <si>
+    <t>Proportion of total removals</t>
+  </si>
+  <si>
+    <t>YPR</t>
+  </si>
+  <si>
+    <t>MPR</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +102,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -93,21 +127,144 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -407,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:T137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="D131" sqref="B130:D131"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="O137" sqref="O137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -421,6 +578,7 @@
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2328,7 +2486,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:20">
       <c r="A97">
         <v>29007</v>
       </c>
@@ -2348,7 +2506,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:20">
       <c r="A98">
         <v>38386</v>
       </c>
@@ -2368,7 +2526,7 @@
         <v>1983</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:20">
       <c r="A99">
         <v>44971</v>
       </c>
@@ -2388,7 +2546,7 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:20">
       <c r="A100">
         <v>57702</v>
       </c>
@@ -2408,7 +2566,7 @@
         <v>1985</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:20">
       <c r="A101">
         <v>72832</v>
       </c>
@@ -2428,7 +2586,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:20">
       <c r="A102">
         <v>72196</v>
       </c>
@@ -2448,7 +2606,7 @@
         <v>1987</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:20">
       <c r="A103">
         <v>76340</v>
       </c>
@@ -2467,8 +2625,11 @@
       <c r="F103">
         <v>1988</v>
       </c>
-    </row>
-    <row r="104" spans="1:6">
+      <c r="Q103" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20">
       <c r="A104">
         <v>68975</v>
       </c>
@@ -2487,8 +2648,32 @@
       <c r="F104">
         <v>1989</v>
       </c>
-    </row>
-    <row r="105" spans="1:6">
+      <c r="L104" t="s">
+        <v>7</v>
+      </c>
+      <c r="M104" t="s">
+        <v>4</v>
+      </c>
+      <c r="N104" t="s">
+        <v>0</v>
+      </c>
+      <c r="O104" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>7</v>
+      </c>
+      <c r="R104" t="s">
+        <v>4</v>
+      </c>
+      <c r="S104" t="s">
+        <v>0</v>
+      </c>
+      <c r="T104" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20">
       <c r="A105">
         <v>63621</v>
       </c>
@@ -2507,8 +2692,40 @@
       <c r="F105">
         <v>1990</v>
       </c>
-    </row>
-    <row r="106" spans="1:6">
+      <c r="L105">
+        <f>SUM(A105:B105)</f>
+        <v>64980</v>
+      </c>
+      <c r="M105" s="1">
+        <f>C105</f>
+        <v>17682</v>
+      </c>
+      <c r="N105" s="1">
+        <f t="shared" ref="N105:O105" si="0">D105</f>
+        <v>5586</v>
+      </c>
+      <c r="O105" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q105">
+        <f>(B105+A105)/SUM($A105:$D105)</f>
+        <v>0.73633396790862116</v>
+      </c>
+      <c r="R105">
+        <f>(C105)/SUM($A105:$E105)</f>
+        <v>0.20036714713081316</v>
+      </c>
+      <c r="S105">
+        <f>(D105)/SUM($A105:$E105)</f>
+        <v>6.3298884960565682E-2</v>
+      </c>
+      <c r="T105">
+        <f>(E105)/SUM($A105:$E105)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20">
       <c r="A106">
         <v>59308</v>
       </c>
@@ -2527,8 +2744,40 @@
       <c r="F106">
         <v>1991</v>
       </c>
-    </row>
-    <row r="107" spans="1:6">
+      <c r="L106">
+        <f t="shared" ref="L106:L129" si="1">SUM(A106:B106)</f>
+        <v>60545</v>
+      </c>
+      <c r="M106" s="1">
+        <f t="shared" ref="M106:M129" si="2">C106</f>
+        <v>19670</v>
+      </c>
+      <c r="N106" s="1">
+        <f t="shared" ref="N106:N129" si="3">D106</f>
+        <v>6509</v>
+      </c>
+      <c r="O106" s="1">
+        <f t="shared" ref="O106:O129" si="4">E106</f>
+        <v>2011</v>
+      </c>
+      <c r="Q106">
+        <f>(B106+A106)/SUM($A106:$D106)</f>
+        <v>0.69813431114800972</v>
+      </c>
+      <c r="R106">
+        <f>(C106)/SUM($A106:$E106)</f>
+        <v>0.22167126838338874</v>
+      </c>
+      <c r="S106">
+        <f>(D106)/SUM($A106:$E106)</f>
+        <v>7.3353242801600271E-2</v>
+      </c>
+      <c r="T106">
+        <f>(E106)/SUM($A106:$E106)</f>
+        <v>2.2662985293289008E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20">
       <c r="A107">
         <v>61145</v>
       </c>
@@ -2547,8 +2796,40 @@
       <c r="F107">
         <v>1992</v>
       </c>
-    </row>
-    <row r="108" spans="1:6">
+      <c r="L107">
+        <f t="shared" si="1"/>
+        <v>62386</v>
+      </c>
+      <c r="M107" s="1">
+        <f t="shared" si="2"/>
+        <v>20293</v>
+      </c>
+      <c r="N107" s="1">
+        <f t="shared" si="3"/>
+        <v>6179</v>
+      </c>
+      <c r="O107" s="1">
+        <f t="shared" si="4"/>
+        <v>1114</v>
+      </c>
+      <c r="Q107">
+        <f>(B107+A107)/SUM($A107:$D107)</f>
+        <v>0.70208647505007993</v>
+      </c>
+      <c r="R107">
+        <f>(C107)/SUM($A107:$E107)</f>
+        <v>0.22554794825056684</v>
+      </c>
+      <c r="S107">
+        <f>(D107)/SUM($A107:$E107)</f>
+        <v>6.867692170897613E-2</v>
+      </c>
+      <c r="T107">
+        <f>(E107)/SUM($A107:$E107)</f>
+        <v>1.238162984039479E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20">
       <c r="A108">
         <v>60087</v>
       </c>
@@ -2567,8 +2848,40 @@
       <c r="F108">
         <v>1993</v>
       </c>
-    </row>
-    <row r="109" spans="1:6">
+      <c r="L108">
+        <f t="shared" si="1"/>
+        <v>61314</v>
+      </c>
+      <c r="M108" s="1">
+        <f t="shared" si="2"/>
+        <v>15964</v>
+      </c>
+      <c r="N108" s="1">
+        <f t="shared" si="3"/>
+        <v>7725</v>
+      </c>
+      <c r="O108" s="1">
+        <f t="shared" si="4"/>
+        <v>933</v>
+      </c>
+      <c r="Q108">
+        <f>(B108+A108)/SUM($A108:$D108)</f>
+        <v>0.72131571826876695</v>
+      </c>
+      <c r="R108">
+        <f>(C108)/SUM($A108:$E108)</f>
+        <v>0.18576615155464532</v>
+      </c>
+      <c r="S108">
+        <f>(D108)/SUM($A108:$E108)</f>
+        <v>8.9892478123254516E-2</v>
+      </c>
+      <c r="T108">
+        <f>(E108)/SUM($A108:$E108)</f>
+        <v>1.0856916775274623E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20">
       <c r="A109">
         <v>56025</v>
       </c>
@@ -2587,8 +2900,40 @@
       <c r="F109">
         <v>1994</v>
       </c>
-    </row>
-    <row r="110" spans="1:6">
+      <c r="L109">
+        <f t="shared" si="1"/>
+        <v>57242</v>
+      </c>
+      <c r="M109" s="1">
+        <f t="shared" si="2"/>
+        <v>16952</v>
+      </c>
+      <c r="N109" s="1">
+        <f t="shared" si="3"/>
+        <v>7065</v>
+      </c>
+      <c r="O109" s="1">
+        <f t="shared" si="4"/>
+        <v>928</v>
+      </c>
+      <c r="Q109">
+        <f>(B109+A109)/SUM($A109:$D109)</f>
+        <v>0.70443889292263007</v>
+      </c>
+      <c r="R109">
+        <f>(C109)/SUM($A109:$E109)</f>
+        <v>0.20626133086741213</v>
+      </c>
+      <c r="S109">
+        <f>(D109)/SUM($A109:$E109)</f>
+        <v>8.5962500152092183E-2</v>
+      </c>
+      <c r="T109">
+        <f>(E109)/SUM($A109:$E109)</f>
+        <v>1.1291323445313736E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20">
       <c r="A110">
         <v>44142</v>
       </c>
@@ -2607,8 +2952,43 @@
       <c r="F110">
         <v>1995</v>
       </c>
-    </row>
-    <row r="111" spans="1:6">
+      <c r="I110" t="s">
+        <v>10</v>
+      </c>
+      <c r="L110">
+        <f t="shared" si="1"/>
+        <v>44814</v>
+      </c>
+      <c r="M110" s="1">
+        <f t="shared" si="2"/>
+        <v>15932</v>
+      </c>
+      <c r="N110" s="1">
+        <f t="shared" si="3"/>
+        <v>7462</v>
+      </c>
+      <c r="O110" s="1">
+        <f t="shared" si="4"/>
+        <v>542</v>
+      </c>
+      <c r="Q110">
+        <f>(B110+A110)/SUM($A110:$D110)</f>
+        <v>0.65701970443349755</v>
+      </c>
+      <c r="R110">
+        <f>(C110)/SUM($A110:$E110)</f>
+        <v>0.23173818181818182</v>
+      </c>
+      <c r="S110">
+        <f>(D110)/SUM($A110:$E110)</f>
+        <v>0.10853818181818181</v>
+      </c>
+      <c r="T110">
+        <f>(E110)/SUM($A110:$E110)</f>
+        <v>7.8836363636363635E-3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20">
       <c r="A111">
         <v>47697</v>
       </c>
@@ -2627,8 +3007,55 @@
       <c r="F111">
         <v>1996</v>
       </c>
-    </row>
-    <row r="112" spans="1:6">
+      <c r="G111" t="s">
+        <v>1</v>
+      </c>
+      <c r="H111" t="s">
+        <v>8</v>
+      </c>
+      <c r="I111" t="s">
+        <v>7</v>
+      </c>
+      <c r="J111" t="s">
+        <v>4</v>
+      </c>
+      <c r="K111" t="s">
+        <v>0</v>
+      </c>
+      <c r="L111">
+        <f t="shared" si="1"/>
+        <v>48497</v>
+      </c>
+      <c r="M111" s="1">
+        <f t="shared" si="2"/>
+        <v>14464</v>
+      </c>
+      <c r="N111" s="1">
+        <f t="shared" si="3"/>
+        <v>8083</v>
+      </c>
+      <c r="O111" s="1">
+        <f t="shared" si="4"/>
+        <v>543</v>
+      </c>
+      <c r="Q111">
+        <f>(B111+A111)/SUM($A111:$D111)</f>
+        <v>0.68263329767468051</v>
+      </c>
+      <c r="R111">
+        <f>(C111)/SUM($A111:$E111)</f>
+        <v>0.20204785785128584</v>
+      </c>
+      <c r="S111">
+        <f>(D111)/SUM($A111:$E111)</f>
+        <v>0.11291156215513989</v>
+      </c>
+      <c r="T111">
+        <f>(E111)/SUM($A111:$E111)</f>
+        <v>7.5851760794557674E-3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20">
       <c r="A112">
         <v>65487</v>
       </c>
@@ -2647,8 +3074,58 @@
       <c r="F112">
         <v>1997</v>
       </c>
-    </row>
-    <row r="113" spans="1:6">
+      <c r="G112">
+        <v>1997</v>
+      </c>
+      <c r="H112">
+        <v>7.7840999999999996</v>
+      </c>
+      <c r="I112">
+        <f>(A112+B112)/(q*$H112)</f>
+        <v>0.19968435785120159</v>
+      </c>
+      <c r="J112">
+        <f>C112/(q*$H112)</f>
+        <v>4.0488787102264077E-2</v>
+      </c>
+      <c r="K112">
+        <f>D112/(q*$H112)</f>
+        <v>2.7041464041880656E-2</v>
+      </c>
+      <c r="L112">
+        <f t="shared" si="1"/>
+        <v>66644</v>
+      </c>
+      <c r="M112" s="1">
+        <f t="shared" si="2"/>
+        <v>13513</v>
+      </c>
+      <c r="N112" s="1">
+        <f t="shared" si="3"/>
+        <v>9025</v>
+      </c>
+      <c r="O112" s="1">
+        <f t="shared" si="4"/>
+        <v>543</v>
+      </c>
+      <c r="Q112">
+        <f>(B112+A112)/SUM($A112:$D112)</f>
+        <v>0.74728084142539974</v>
+      </c>
+      <c r="R112">
+        <f>(C112)/SUM($A112:$E112)</f>
+        <v>0.1506046252438005</v>
+      </c>
+      <c r="S112">
+        <f>(D112)/SUM($A112:$E112)</f>
+        <v>0.10058512120367791</v>
+      </c>
+      <c r="T112">
+        <f>(E112)/SUM($A112:$E112)</f>
+        <v>6.0518250208971862E-3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20">
       <c r="A113">
         <v>70127</v>
       </c>
@@ -2667,8 +3144,58 @@
       <c r="F113">
         <v>1998</v>
       </c>
-    </row>
-    <row r="114" spans="1:6">
+      <c r="G113">
+        <v>1998</v>
+      </c>
+      <c r="H113">
+        <v>6.9726999999999997</v>
+      </c>
+      <c r="I113">
+        <f>(A113+B113)/(q*$H113)</f>
+        <v>0.23907738919887081</v>
+      </c>
+      <c r="J113">
+        <f>C113/(q*$H113)</f>
+        <v>4.4012931794481097E-2</v>
+      </c>
+      <c r="K113">
+        <f>D113/(q*$H113)</f>
+        <v>2.8719792703101894E-2</v>
+      </c>
+      <c r="L113">
+        <f t="shared" si="1"/>
+        <v>71474</v>
+      </c>
+      <c r="M113" s="1">
+        <f t="shared" si="2"/>
+        <v>13158</v>
+      </c>
+      <c r="N113" s="1">
+        <f t="shared" si="3"/>
+        <v>8586</v>
+      </c>
+      <c r="O113" s="1">
+        <f t="shared" si="4"/>
+        <v>740</v>
+      </c>
+      <c r="Q113">
+        <f>(B113+A113)/SUM($A113:$D113)</f>
+        <v>0.76674032912098522</v>
+      </c>
+      <c r="R113">
+        <f>(C113)/SUM($A113:$E113)</f>
+        <v>0.140041295046723</v>
+      </c>
+      <c r="S113">
+        <f>(D113)/SUM($A113:$E113)</f>
+        <v>9.1381255454564811E-2</v>
+      </c>
+      <c r="T113">
+        <f>(E113)/SUM($A113:$E113)</f>
+        <v>7.875859426552289E-3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20">
       <c r="A114">
         <v>74705</v>
       </c>
@@ -2687,8 +3214,58 @@
       <c r="F114">
         <v>1999</v>
       </c>
-    </row>
-    <row r="115" spans="1:6">
+      <c r="G114">
+        <v>1999</v>
+      </c>
+      <c r="H114">
+        <v>6.2648999999999999</v>
+      </c>
+      <c r="I114">
+        <f>(A114+B114)/(q*$H114)</f>
+        <v>0.28276646588142235</v>
+      </c>
+      <c r="J114">
+        <f>C114/(q*$H114)</f>
+        <v>5.0422479578402506E-2</v>
+      </c>
+      <c r="K114">
+        <f>D114/(q*$H114)</f>
+        <v>2.7471018665758424E-2</v>
+      </c>
+      <c r="L114">
+        <f t="shared" si="1"/>
+        <v>75954</v>
+      </c>
+      <c r="M114" s="1">
+        <f t="shared" si="2"/>
+        <v>13544</v>
+      </c>
+      <c r="N114" s="1">
+        <f t="shared" si="3"/>
+        <v>7379</v>
+      </c>
+      <c r="O114" s="1">
+        <f t="shared" si="4"/>
+        <v>745</v>
+      </c>
+      <c r="Q114">
+        <f>(B114+A114)/SUM($A114:$D114)</f>
+        <v>0.78402510399785297</v>
+      </c>
+      <c r="R114">
+        <f>(C114)/SUM($A114:$E114)</f>
+        <v>0.13873921861875396</v>
+      </c>
+      <c r="S114">
+        <f>(D114)/SUM($A114:$E114)</f>
+        <v>7.5587470037491555E-2</v>
+      </c>
+      <c r="T114">
+        <f>(E114)/SUM($A114:$E114)</f>
+        <v>7.6314765114420926E-3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20">
       <c r="A115">
         <v>68560</v>
       </c>
@@ -2707,8 +3284,58 @@
       <c r="F115">
         <v>2000</v>
       </c>
-    </row>
-    <row r="116" spans="1:6">
+      <c r="G115">
+        <v>2000</v>
+      </c>
+      <c r="H115">
+        <v>6.6265000000000001</v>
+      </c>
+      <c r="I115">
+        <f>(A115+B115)/(q*$H115)</f>
+        <v>0.24547531115588125</v>
+      </c>
+      <c r="J115">
+        <f>C115/(q*$H115)</f>
+        <v>4.5833696598538719E-2</v>
+      </c>
+      <c r="K115">
+        <f>D115/(q*$H115)</f>
+        <v>3.1709090205516453E-2</v>
+      </c>
+      <c r="L115">
+        <f t="shared" si="1"/>
+        <v>69743</v>
+      </c>
+      <c r="M115" s="1">
+        <f t="shared" si="2"/>
+        <v>13022</v>
+      </c>
+      <c r="N115" s="1">
+        <f t="shared" si="3"/>
+        <v>9009</v>
+      </c>
+      <c r="O115" s="1">
+        <f t="shared" si="4"/>
+        <v>757</v>
+      </c>
+      <c r="Q115">
+        <f>(B115+A115)/SUM($A115:$D115)</f>
+        <v>0.75994290321877656</v>
+      </c>
+      <c r="R115">
+        <f>(C115)/SUM($A115:$E115)</f>
+        <v>0.14073121440382141</v>
+      </c>
+      <c r="S115">
+        <f>(D115)/SUM($A115:$E115)</f>
+        <v>9.7361965179237231E-2</v>
+      </c>
+      <c r="T115">
+        <f>(E115)/SUM($A115:$E115)</f>
+        <v>8.1810420291577955E-3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20">
       <c r="A116">
         <v>70980</v>
       </c>
@@ -2727,8 +3354,58 @@
       <c r="F116">
         <v>2001</v>
       </c>
-    </row>
-    <row r="117" spans="1:6">
+      <c r="G116">
+        <v>2001</v>
+      </c>
+      <c r="H116">
+        <v>6.3841999999999999</v>
+      </c>
+      <c r="I116">
+        <f>(A116+B116)/(q*$H116)</f>
+        <v>0.26445116900008186</v>
+      </c>
+      <c r="J116">
+        <f>C116/(q*$H116)</f>
+        <v>4.7036191593463665E-2</v>
+      </c>
+      <c r="K116">
+        <f>D116/(q*$H116)</f>
+        <v>2.960631430473239E-2</v>
+      </c>
+      <c r="L116">
+        <f t="shared" si="1"/>
+        <v>72387</v>
+      </c>
+      <c r="M116" s="1">
+        <f t="shared" si="2"/>
+        <v>12875</v>
+      </c>
+      <c r="N116" s="1">
+        <f t="shared" si="3"/>
+        <v>8104</v>
+      </c>
+      <c r="O116" s="1">
+        <f t="shared" si="4"/>
+        <v>772</v>
+      </c>
+      <c r="Q116">
+        <f>(B116+A116)/SUM($A116:$D116)</f>
+        <v>0.7753036437246964</v>
+      </c>
+      <c r="R116">
+        <f>(C116)/SUM($A116:$E116)</f>
+        <v>0.13676729907157578</v>
+      </c>
+      <c r="S116">
+        <f>(D116)/SUM($A116:$E116)</f>
+        <v>8.6086383819499027E-2</v>
+      </c>
+      <c r="T116">
+        <f>(E116)/SUM($A116:$E116)</f>
+        <v>8.2007265928742915E-3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20">
       <c r="A117">
         <v>74957</v>
       </c>
@@ -2747,8 +3424,58 @@
       <c r="F117">
         <v>2002</v>
       </c>
-    </row>
-    <row r="118" spans="1:6">
+      <c r="G117">
+        <v>2002</v>
+      </c>
+      <c r="H117">
+        <v>6.3893000000000004</v>
+      </c>
+      <c r="I117">
+        <f>(A117+B117)/(q*$H117)</f>
+        <v>0.27881605025460526</v>
+      </c>
+      <c r="J117">
+        <f>C117/(q*$H117)</f>
+        <v>4.5005539193362504E-2</v>
+      </c>
+      <c r="K117">
+        <f>D117/(q*$H117)</f>
+        <v>2.9246847272059402E-2</v>
+      </c>
+      <c r="L117">
+        <f t="shared" si="1"/>
+        <v>76380</v>
+      </c>
+      <c r="M117" s="1">
+        <f t="shared" si="2"/>
+        <v>12329</v>
+      </c>
+      <c r="N117" s="1">
+        <f t="shared" si="3"/>
+        <v>8012</v>
+      </c>
+      <c r="O117" s="1">
+        <f t="shared" si="4"/>
+        <v>771</v>
+      </c>
+      <c r="Q117">
+        <f>(B117+A117)/SUM($A117:$D117)</f>
+        <v>0.78969406850632229</v>
+      </c>
+      <c r="R117">
+        <f>(C117)/SUM($A117:$E117)</f>
+        <v>0.12646165839248349</v>
+      </c>
+      <c r="S117">
+        <f>(D117)/SUM($A117:$E117)</f>
+        <v>8.2181102039141668E-2</v>
+      </c>
+      <c r="T117">
+        <f>(E117)/SUM($A117:$E117)</f>
+        <v>7.9083411972264393E-3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20">
       <c r="A118">
         <v>73370</v>
       </c>
@@ -2767,8 +3494,58 @@
       <c r="F118">
         <v>2003</v>
       </c>
-    </row>
-    <row r="119" spans="1:6">
+      <c r="G118">
+        <v>2003</v>
+      </c>
+      <c r="H118">
+        <v>5.7876000000000003</v>
+      </c>
+      <c r="I118">
+        <f>(A118+B118)/(q*$H118)</f>
+        <v>0.30313214426611823</v>
+      </c>
+      <c r="J118">
+        <f>C118/(q*$H118)</f>
+        <v>4.9599851525868877E-2</v>
+      </c>
+      <c r="K118">
+        <f>D118/(q*$H118)</f>
+        <v>3.7667355558360122E-2</v>
+      </c>
+      <c r="L118">
+        <f t="shared" si="1"/>
+        <v>75221</v>
+      </c>
+      <c r="M118" s="1">
+        <f t="shared" si="2"/>
+        <v>12308</v>
+      </c>
+      <c r="N118" s="1">
+        <f t="shared" si="3"/>
+        <v>9347</v>
+      </c>
+      <c r="O118" s="1">
+        <f t="shared" si="4"/>
+        <v>1376</v>
+      </c>
+      <c r="Q118">
+        <f>(B118+A118)/SUM($A118:$D118)</f>
+        <v>0.77646682356827279</v>
+      </c>
+      <c r="R118">
+        <f>(C118)/SUM($A118:$E118)</f>
+        <v>0.1252697146114074</v>
+      </c>
+      <c r="S118">
+        <f>(D118)/SUM($A118:$E118)</f>
+        <v>9.5132923502829453E-2</v>
+      </c>
+      <c r="T118">
+        <f>(E118)/SUM($A118:$E118)</f>
+        <v>1.4004803973456012E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20">
       <c r="A119">
         <v>73314</v>
       </c>
@@ -2787,8 +3564,58 @@
       <c r="F119">
         <v>2004</v>
       </c>
-    </row>
-    <row r="120" spans="1:6">
+      <c r="G119">
+        <v>2004</v>
+      </c>
+      <c r="H119">
+        <v>6.4579000000000004</v>
+      </c>
+      <c r="I119">
+        <f>(A119+B119)/(q*$H119)</f>
+        <v>0.27236547632330377</v>
+      </c>
+      <c r="J119">
+        <f>C119/(q*$H119)</f>
+        <v>4.4386608640483244E-2</v>
+      </c>
+      <c r="K119">
+        <f>D119/(q*$H119)</f>
+        <v>3.865499367608561E-2</v>
+      </c>
+      <c r="L119">
+        <f t="shared" si="1"/>
+        <v>75414</v>
+      </c>
+      <c r="M119" s="1">
+        <f t="shared" si="2"/>
+        <v>12290</v>
+      </c>
+      <c r="N119" s="1">
+        <f t="shared" si="3"/>
+        <v>10703</v>
+      </c>
+      <c r="O119" s="1">
+        <f t="shared" si="4"/>
+        <v>1548</v>
+      </c>
+      <c r="Q119">
+        <f>(B119+A119)/SUM($A119:$D119)</f>
+        <v>0.76634792240389404</v>
+      </c>
+      <c r="R119">
+        <f>(C119)/SUM($A119:$E119)</f>
+        <v>0.1229553298984543</v>
+      </c>
+      <c r="S119">
+        <f>(D119)/SUM($A119:$E119)</f>
+        <v>0.10707818518333249</v>
+      </c>
+      <c r="T119">
+        <f>(E119)/SUM($A119:$E119)</f>
+        <v>1.548696913611125E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20">
       <c r="A120">
         <v>72111</v>
       </c>
@@ -2807,8 +3634,58 @@
       <c r="F120">
         <v>2005</v>
       </c>
-    </row>
-    <row r="121" spans="1:6">
+      <c r="G120">
+        <v>2005</v>
+      </c>
+      <c r="H120">
+        <v>5.9282000000000004</v>
+      </c>
+      <c r="I120">
+        <f>(A120+B120)/(q*$H120)</f>
+        <v>0.29128842573042402</v>
+      </c>
+      <c r="J120">
+        <f>C120/(q*$H120)</f>
+        <v>5.1027997538069636E-2</v>
+      </c>
+      <c r="K120">
+        <f>D120/(q*$H120)</f>
+        <v>4.2722669642706108E-2</v>
+      </c>
+      <c r="L120">
+        <f t="shared" si="1"/>
+        <v>74038</v>
+      </c>
+      <c r="M120" s="1">
+        <f t="shared" si="2"/>
+        <v>12970</v>
+      </c>
+      <c r="N120" s="1">
+        <f t="shared" si="3"/>
+        <v>10859</v>
+      </c>
+      <c r="O120" s="1">
+        <f t="shared" si="4"/>
+        <v>1537</v>
+      </c>
+      <c r="Q120">
+        <f>(B120+A120)/SUM($A120:$D120)</f>
+        <v>0.7565164968784166</v>
+      </c>
+      <c r="R120">
+        <f>(C120)/SUM($A120:$E120)</f>
+        <v>0.13047764677477766</v>
+      </c>
+      <c r="S120">
+        <f>(D120)/SUM($A120:$E120)</f>
+        <v>0.10924107681783429</v>
+      </c>
+      <c r="T120">
+        <f>(E120)/SUM($A120:$E120)</f>
+        <v>1.5462154440465172E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20">
       <c r="A121">
         <v>68125</v>
       </c>
@@ -2827,8 +3704,58 @@
       <c r="F121">
         <v>2006</v>
       </c>
-    </row>
-    <row r="122" spans="1:6">
+      <c r="G121">
+        <v>2006</v>
+      </c>
+      <c r="H121">
+        <v>5.4306000000000001</v>
+      </c>
+      <c r="I121">
+        <f>(A121+B121)/(q*$H121)</f>
+        <v>0.30253904024273381</v>
+      </c>
+      <c r="J121">
+        <f>C121/(q*$H121)</f>
+        <v>5.4943457005313424E-2</v>
+      </c>
+      <c r="K121">
+        <f>D121/(q*$H121)</f>
+        <v>4.3768371010798807E-2</v>
+      </c>
+      <c r="L121">
+        <f t="shared" si="1"/>
+        <v>70443</v>
+      </c>
+      <c r="M121" s="1">
+        <f t="shared" si="2"/>
+        <v>12793</v>
+      </c>
+      <c r="N121" s="1">
+        <f t="shared" si="3"/>
+        <v>10191</v>
+      </c>
+      <c r="O121" s="1">
+        <f t="shared" si="4"/>
+        <v>1481</v>
+      </c>
+      <c r="Q121">
+        <f>(B121+A121)/SUM($A121:$D121)</f>
+        <v>0.75398974600490221</v>
+      </c>
+      <c r="R121">
+        <f>(C121)/SUM($A121:$E121)</f>
+        <v>0.13479369494668522</v>
+      </c>
+      <c r="S121">
+        <f>(D121)/SUM($A121:$E121)</f>
+        <v>0.10737767100771273</v>
+      </c>
+      <c r="T121">
+        <f>(E121)/SUM($A121:$E121)</f>
+        <v>1.5604585493319846E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20">
       <c r="A122">
         <v>63032</v>
       </c>
@@ -2847,8 +3774,58 @@
       <c r="F122">
         <v>2007</v>
       </c>
-    </row>
-    <row r="123" spans="1:6">
+      <c r="G122">
+        <v>2007</v>
+      </c>
+      <c r="H122">
+        <v>5.7267000000000001</v>
+      </c>
+      <c r="I122">
+        <f>(A122+B122)/(q*$H122)</f>
+        <v>0.26659765841756311</v>
+      </c>
+      <c r="J122">
+        <f>C122/(q*$H122)</f>
+        <v>4.8828111134728062E-2</v>
+      </c>
+      <c r="K122">
+        <f>D122/(q*$H122)</f>
+        <v>4.6677703037377456E-2</v>
+      </c>
+      <c r="L122">
+        <f t="shared" si="1"/>
+        <v>65459</v>
+      </c>
+      <c r="M122" s="1">
+        <f t="shared" si="2"/>
+        <v>11989</v>
+      </c>
+      <c r="N122" s="1">
+        <f t="shared" si="3"/>
+        <v>11461</v>
+      </c>
+      <c r="O122" s="1">
+        <f t="shared" si="4"/>
+        <v>1486</v>
+      </c>
+      <c r="Q122">
+        <f>(B122+A122)/SUM($A122:$D122)</f>
+        <v>0.73624717407686513</v>
+      </c>
+      <c r="R122">
+        <f>(C122)/SUM($A122:$E122)</f>
+        <v>0.13262901709165331</v>
+      </c>
+      <c r="S122">
+        <f>(D122)/SUM($A122:$E122)</f>
+        <v>0.12678798606117594</v>
+      </c>
+      <c r="T122">
+        <f>(E122)/SUM($A122:$E122)</f>
+        <v>1.643896233198739E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20">
       <c r="A123">
         <v>58706</v>
       </c>
@@ -2867,8 +3844,58 @@
       <c r="F123">
         <v>2008</v>
       </c>
-    </row>
-    <row r="124" spans="1:6">
+      <c r="G123">
+        <v>2008</v>
+      </c>
+      <c r="H123">
+        <v>5.6536</v>
+      </c>
+      <c r="I123">
+        <f>(A123+B123)/(q*$H123)</f>
+        <v>0.25300267934326398</v>
+      </c>
+      <c r="J123">
+        <f>C123/(q*$H123)</f>
+        <v>4.7862918825667698E-2</v>
+      </c>
+      <c r="K123">
+        <f>D123/(q*$H123)</f>
+        <v>4.4030419981585189E-2</v>
+      </c>
+      <c r="L123">
+        <f t="shared" si="1"/>
+        <v>61328</v>
+      </c>
+      <c r="M123" s="1">
+        <f t="shared" si="2"/>
+        <v>11602</v>
+      </c>
+      <c r="N123" s="1">
+        <f t="shared" si="3"/>
+        <v>10673</v>
+      </c>
+      <c r="O123" s="1">
+        <f t="shared" si="4"/>
+        <v>1344</v>
+      </c>
+      <c r="Q123">
+        <f>(B123+A123)/SUM($A123:$D123)</f>
+        <v>0.73356219274427947</v>
+      </c>
+      <c r="R123">
+        <f>(C123)/SUM($A123:$E123)</f>
+        <v>0.13657927884445595</v>
+      </c>
+      <c r="S123">
+        <f>(D123)/SUM($A123:$E123)</f>
+        <v>0.12564304801817605</v>
+      </c>
+      <c r="T123">
+        <f>(E123)/SUM($A123:$E123)</f>
+        <v>1.5821629957502914E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:20">
       <c r="A124">
         <v>52176</v>
       </c>
@@ -2887,8 +3914,58 @@
       <c r="F124">
         <v>2009</v>
       </c>
-    </row>
-    <row r="125" spans="1:6">
+      <c r="G124">
+        <v>2009</v>
+      </c>
+      <c r="H124">
+        <v>5.4951999999999996</v>
+      </c>
+      <c r="I124">
+        <f>(A124+B124)/(q*$H124)</f>
+        <v>0.23339079072583607</v>
+      </c>
+      <c r="J124">
+        <f>C124/(q*$H124)</f>
+        <v>4.7039774020521216E-2</v>
+      </c>
+      <c r="K124">
+        <f>D124/(q*$H124)</f>
+        <v>3.727784311307749E-2</v>
+      </c>
+      <c r="L124">
+        <f t="shared" si="1"/>
+        <v>54989</v>
+      </c>
+      <c r="M124" s="1">
+        <f t="shared" si="2"/>
+        <v>11083</v>
+      </c>
+      <c r="N124" s="1">
+        <f t="shared" si="3"/>
+        <v>8783</v>
+      </c>
+      <c r="O124" s="1">
+        <f t="shared" si="4"/>
+        <v>1308</v>
+      </c>
+      <c r="Q124">
+        <f>(B124+A124)/SUM($A124:$D124)</f>
+        <v>0.73460690668626005</v>
+      </c>
+      <c r="R124">
+        <f>(C124)/SUM($A124:$E124)</f>
+        <v>0.14551685201475781</v>
+      </c>
+      <c r="S124">
+        <f>(D124)/SUM($A124:$E124)</f>
+        <v>0.11531846172025786</v>
+      </c>
+      <c r="T124">
+        <f>(E124)/SUM($A124:$E124)</f>
+        <v>1.7173693263133016E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20">
       <c r="A125">
         <v>49825</v>
       </c>
@@ -2907,8 +3984,58 @@
       <c r="F125">
         <v>2010</v>
       </c>
-    </row>
-    <row r="126" spans="1:6">
+      <c r="G125">
+        <v>2010</v>
+      </c>
+      <c r="H125">
+        <v>5.1238999999999999</v>
+      </c>
+      <c r="I125">
+        <f>(A125+B125)/(q*$H125)</f>
+        <v>0.24091732347373335</v>
+      </c>
+      <c r="J125">
+        <f>C125/(q*$H125)</f>
+        <v>4.7102848514107974E-2</v>
+      </c>
+      <c r="K125">
+        <f>D125/(q*$H125)</f>
+        <v>3.5718598017994325E-2</v>
+      </c>
+      <c r="L125">
+        <f t="shared" si="1"/>
+        <v>52927</v>
+      </c>
+      <c r="M125" s="1">
+        <f t="shared" si="2"/>
+        <v>10348</v>
+      </c>
+      <c r="N125" s="1">
+        <f t="shared" si="3"/>
+        <v>7847</v>
+      </c>
+      <c r="O125" s="1">
+        <f t="shared" si="4"/>
+        <v>1239</v>
+      </c>
+      <c r="Q125">
+        <f>(B125+A125)/SUM($A125:$D125)</f>
+        <v>0.74417198616461855</v>
+      </c>
+      <c r="R125">
+        <f>(C125)/SUM($A125:$E125)</f>
+        <v>0.14300520998880611</v>
+      </c>
+      <c r="S125">
+        <f>(D125)/SUM($A125:$E125)</f>
+        <v>0.10844239300175509</v>
+      </c>
+      <c r="T125">
+        <f>(E125)/SUM($A125:$E125)</f>
+        <v>1.7122483105540279E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20">
       <c r="A126">
         <v>39615</v>
       </c>
@@ -2927,8 +4054,58 @@
       <c r="F126">
         <v>2011</v>
       </c>
-    </row>
-    <row r="127" spans="1:6">
+      <c r="G126">
+        <v>2011</v>
+      </c>
+      <c r="H126">
+        <v>5.0434999999999999</v>
+      </c>
+      <c r="I126">
+        <f>(A126+B126)/(q*$H126)</f>
+        <v>0.19410634406901456</v>
+      </c>
+      <c r="J126">
+        <f>C126/(q*$H126)</f>
+        <v>4.3543749362792226E-2</v>
+      </c>
+      <c r="K126">
+        <f>D126/(q*$H126)</f>
+        <v>3.2847414159294097E-2</v>
+      </c>
+      <c r="L126">
+        <f t="shared" si="1"/>
+        <v>41974</v>
+      </c>
+      <c r="M126" s="1">
+        <f t="shared" si="2"/>
+        <v>9416</v>
+      </c>
+      <c r="N126" s="1">
+        <f t="shared" si="3"/>
+        <v>7103</v>
+      </c>
+      <c r="O126" s="1">
+        <f t="shared" si="4"/>
+        <v>1144</v>
+      </c>
+      <c r="Q126">
+        <f>(B126+A126)/SUM($A126:$D126)</f>
+        <v>0.71759013899099033</v>
+      </c>
+      <c r="R126">
+        <f>(C126)/SUM($A126:$E126)</f>
+        <v>0.15788855911598504</v>
+      </c>
+      <c r="S126">
+        <f>(D126)/SUM($A126:$E126)</f>
+        <v>0.11910391200093902</v>
+      </c>
+      <c r="T126">
+        <f>(E126)/SUM($A126:$E126)</f>
+        <v>1.9182722135586968E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20">
       <c r="A127">
         <v>32052</v>
       </c>
@@ -2947,8 +4124,58 @@
       <c r="F127">
         <v>2012</v>
       </c>
-    </row>
-    <row r="128" spans="1:6">
+      <c r="G127">
+        <v>2012</v>
+      </c>
+      <c r="H127">
+        <v>5.5606</v>
+      </c>
+      <c r="I127">
+        <f>(A127+B127)/(q*$H127)</f>
+        <v>0.14115830405116331</v>
+      </c>
+      <c r="J127">
+        <f>C127/(q*$H127)</f>
+        <v>4.2376013128570242E-2</v>
+      </c>
+      <c r="K127">
+        <f>D127/(q*$H127)</f>
+        <v>2.8404470049161409E-2</v>
+      </c>
+      <c r="L127">
+        <f t="shared" si="1"/>
+        <v>33654</v>
+      </c>
+      <c r="M127" s="1">
+        <f t="shared" si="2"/>
+        <v>10103</v>
+      </c>
+      <c r="N127" s="1">
+        <f t="shared" si="3"/>
+        <v>6772</v>
+      </c>
+      <c r="O127" s="1">
+        <f t="shared" si="4"/>
+        <v>1140</v>
+      </c>
+      <c r="Q127">
+        <f>(B127+A127)/SUM($A127:$D127)</f>
+        <v>0.66603336697737936</v>
+      </c>
+      <c r="R127">
+        <f>(C127)/SUM($A127:$E127)</f>
+        <v>0.19553310495655035</v>
+      </c>
+      <c r="S127">
+        <f>(D127)/SUM($A127:$E127)</f>
+        <v>0.13106504867522112</v>
+      </c>
+      <c r="T127">
+        <f>(E127)/SUM($A127:$E127)</f>
+        <v>2.2063519712013004E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20">
       <c r="A128">
         <v>29126</v>
       </c>
@@ -2967,8 +4194,58 @@
       <c r="F128">
         <v>2013</v>
       </c>
-    </row>
-    <row r="129" spans="1:6">
+      <c r="G128">
+        <v>2013</v>
+      </c>
+      <c r="H128">
+        <v>4.7301000000000002</v>
+      </c>
+      <c r="I128">
+        <f>(A128+B128)/(q*$H128)</f>
+        <v>0.15025261325319922</v>
+      </c>
+      <c r="J128">
+        <f>C128/(q*$H128)</f>
+        <v>4.3593572911903855E-2</v>
+      </c>
+      <c r="K128">
+        <f>D128/(q*$H128)</f>
+        <v>3.7415228057405998E-2</v>
+      </c>
+      <c r="L128">
+        <f t="shared" si="1"/>
+        <v>30472</v>
+      </c>
+      <c r="M128" s="1">
+        <f t="shared" si="2"/>
+        <v>8841</v>
+      </c>
+      <c r="N128" s="1">
+        <f t="shared" si="3"/>
+        <v>7588</v>
+      </c>
+      <c r="O128" s="1">
+        <f t="shared" si="4"/>
+        <v>1137</v>
+      </c>
+      <c r="Q128">
+        <f>(B128+A128)/SUM($A128:$D128)</f>
+        <v>0.64970896142939383</v>
+      </c>
+      <c r="R128">
+        <f>(C128)/SUM($A128:$E128)</f>
+        <v>0.18404180024147551</v>
+      </c>
+      <c r="S128">
+        <f>(D128)/SUM($A128:$E128)</f>
+        <v>0.15795828302593781</v>
+      </c>
+      <c r="T128">
+        <f>(E128)/SUM($A128:$E128)</f>
+        <v>2.3668762229901327E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20">
       <c r="A129">
         <v>23739</v>
       </c>
@@ -2987,8 +4264,58 @@
       <c r="F129">
         <v>2014</v>
       </c>
-    </row>
-    <row r="130" spans="1:6">
+      <c r="G129">
+        <v>2014</v>
+      </c>
+      <c r="H129">
+        <v>5.1645000000000003</v>
+      </c>
+      <c r="I129">
+        <f>(A129+B129)/(q*$H129)</f>
+        <v>0.11279851675712529</v>
+      </c>
+      <c r="J129">
+        <f>C129/(q*$H129)</f>
+        <v>4.2067429378733319E-2</v>
+      </c>
+      <c r="K129">
+        <f>D129/(q*$H129)</f>
+        <v>3.1987504271558574E-2</v>
+      </c>
+      <c r="L129">
+        <f t="shared" si="1"/>
+        <v>24977</v>
+      </c>
+      <c r="M129" s="1">
+        <f t="shared" si="2"/>
+        <v>9315</v>
+      </c>
+      <c r="N129" s="1">
+        <f t="shared" si="3"/>
+        <v>7083</v>
+      </c>
+      <c r="O129" s="1">
+        <f t="shared" si="4"/>
+        <v>1137</v>
+      </c>
+      <c r="Q129">
+        <f>(B129+A129)/SUM($A129:$D129)</f>
+        <v>0.60367371601208464</v>
+      </c>
+      <c r="R129">
+        <f>(C129)/SUM($A129:$E129)</f>
+        <v>0.21911460293564169</v>
+      </c>
+      <c r="S129">
+        <f>(D129)/SUM($A129:$E129)</f>
+        <v>0.16661178020323672</v>
+      </c>
+      <c r="T129">
+        <f>(E129)/SUM($A129:$E129)</f>
+        <v>2.6745389537071885E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:20">
       <c r="B130" t="s">
         <v>7</v>
       </c>
@@ -2998,8 +4325,11 @@
       <c r="D130" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:6">
+      <c r="E130" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="131" spans="1:20">
       <c r="B131">
         <f>A129+B129</f>
         <v>24977</v>
@@ -3011,6 +4341,130 @@
       <c r="D131">
         <f>D129</f>
         <v>7083</v>
+      </c>
+      <c r="E131">
+        <f>E129</f>
+        <v>1137</v>
+      </c>
+      <c r="G131" t="s">
+        <v>9</v>
+      </c>
+      <c r="H131">
+        <v>42875.441305157903</v>
+      </c>
+      <c r="L131" s="2">
+        <f>AVERAGE(L105:L129)</f>
+        <v>59730.239999999998</v>
+      </c>
+      <c r="M131" s="2">
+        <f t="shared" ref="M131:O131" si="5">AVERAGE(M105:M129)</f>
+        <v>13298.24</v>
+      </c>
+      <c r="N131" s="2">
+        <f t="shared" si="5"/>
+        <v>8285.36</v>
+      </c>
+      <c r="O131" s="2">
+        <f t="shared" si="5"/>
+        <v>1051.04</v>
+      </c>
+      <c r="Q131" s="3">
+        <f>AVERAGE(Q105:Q129)</f>
+        <v>0.7265545875735071</v>
+      </c>
+      <c r="R131" s="3">
+        <f t="shared" ref="R131:T131" si="6">AVERAGE(R105:R129)</f>
+        <v>0.1653820003221641</v>
+      </c>
+      <c r="S131" s="3">
+        <f t="shared" si="6"/>
+        <v>0.10422311354687325</v>
+      </c>
+      <c r="T131" s="3">
+        <f t="shared" si="6"/>
+        <v>1.3491464555664136E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:20">
+      <c r="B132">
+        <f>B131/SUM($B$131:$E$131)</f>
+        <v>0.58752822732404963</v>
+      </c>
+      <c r="C132">
+        <f t="shared" ref="C132:E132" si="7">C131/SUM($B$131:$E$131)</f>
+        <v>0.21911460293564169</v>
+      </c>
+      <c r="D132">
+        <f t="shared" si="7"/>
+        <v>0.16661178020323672</v>
+      </c>
+      <c r="E132">
+        <f t="shared" si="7"/>
+        <v>2.6745389537071885E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:20">
+      <c r="N133" t="s">
+        <v>13</v>
+      </c>
+      <c r="O133" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20">
+      <c r="L134" t="s">
+        <v>7</v>
+      </c>
+      <c r="M134" s="1">
+        <v>59730.239999999998</v>
+      </c>
+      <c r="N134">
+        <v>0.7265545875735071</v>
+      </c>
+      <c r="O134">
+        <v>0.357678157</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20">
+      <c r="L135" t="s">
+        <v>4</v>
+      </c>
+      <c r="M135" s="1">
+        <v>13298.24</v>
+      </c>
+      <c r="N135">
+        <v>0.1653820003221641</v>
+      </c>
+      <c r="O135">
+        <v>0.54271501099999997</v>
+      </c>
+    </row>
+    <row r="136" spans="1:20">
+      <c r="L136" t="s">
+        <v>0</v>
+      </c>
+      <c r="M136" s="1">
+        <v>8285.36</v>
+      </c>
+      <c r="N136">
+        <v>0.10422311354687325</v>
+      </c>
+      <c r="O136">
+        <v>9.1203046999999995E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:20">
+      <c r="L137" t="s">
+        <v>11</v>
+      </c>
+      <c r="M137" s="1">
+        <v>1051.04</v>
+      </c>
+      <c r="N137">
+        <v>1.3491464555664136E-2</v>
+      </c>
+      <c r="O137">
+        <v>8.4037850000000004E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new files for TMA app
</commit_message>
<xml_diff>
--- a/src/dashboard/data/harvestPolicy/DataFromIan/Removals.xlsx
+++ b/src/dashboard/data/harvestPolicy/DataFromIan/Removals.xlsx
@@ -127,8 +127,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="65">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -200,7 +204,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="65">
+  <cellStyles count="69">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -233,6 +237,8 @@
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -265,6 +271,8 @@
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -567,7 +575,7 @@
   <dimension ref="A1:T137"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="O137" sqref="O137"/>
+      <selection activeCell="O134" sqref="O134:O137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Added option to allow for a fixed PSC limit. Still need to test, and clean up code for output
</commit_message>
<xml_diff>
--- a/src/dashboard/data/harvestPolicy/DataFromIan/Removals.xlsx
+++ b/src/dashboard/data/harvestPolicy/DataFromIan/Removals.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="50640" windowHeight="15500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="q">Sheet1!$H$131</definedName>
   </definedNames>
-  <calcPr calcId="140001" calcMode="autoNoTable" iterate="1" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
   <si>
     <t>Sport</t>
   </si>
@@ -70,13 +70,20 @@
   <si>
     <t>MPR</t>
   </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>5yr Avg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -127,7 +134,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -197,14 +204,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="69">
+  <cellStyles count="83">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -239,6 +261,13 @@
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -273,6 +302,13 @@
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -283,6 +319,267 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$111</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>48497</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$112:$H$129</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>7.784099999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9727</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2649</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.6265</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.3842</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3893</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.7876</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.4579</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.9282</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.4306</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.7267</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.6536</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.4952</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.1239</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.0435</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.5606</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.7301</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.1645</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$112:$L$129</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>66644.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>71474.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75954.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>69743.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>72387.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>76380.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75221.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>75414.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>74038.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>70443.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65459.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>61328.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>54989.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>52927.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41974.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>33654.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>30472.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>24977.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2139200936"/>
+        <c:axId val="2139237176"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2139200936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2139237176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2139237176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2139200936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1079500</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -574,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="O134" sqref="O134:O137"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="I140" sqref="I140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -587,6 +884,7 @@
     <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.83203125" style="1"/>
+    <col min="17" max="20" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2717,19 +3015,19 @@
         <v>0</v>
       </c>
       <c r="Q105">
-        <f>(B105+A105)/SUM($A105:$D105)</f>
+        <f t="shared" ref="Q105:Q129" si="1">(B105+A105)/SUM($A105:$D105)</f>
         <v>0.73633396790862116</v>
       </c>
       <c r="R105">
-        <f>(C105)/SUM($A105:$E105)</f>
+        <f t="shared" ref="R105:R129" si="2">(C105)/SUM($A105:$E105)</f>
         <v>0.20036714713081316</v>
       </c>
       <c r="S105">
-        <f>(D105)/SUM($A105:$E105)</f>
+        <f t="shared" ref="S105:S129" si="3">(D105)/SUM($A105:$E105)</f>
         <v>6.3298884960565682E-2</v>
       </c>
       <c r="T105">
-        <f>(E105)/SUM($A105:$E105)</f>
+        <f t="shared" ref="T105:T129" si="4">(E105)/SUM($A105:$E105)</f>
         <v>0</v>
       </c>
     </row>
@@ -2753,35 +3051,35 @@
         <v>1991</v>
       </c>
       <c r="L106">
-        <f t="shared" ref="L106:L129" si="1">SUM(A106:B106)</f>
+        <f t="shared" ref="L106:L129" si="5">SUM(A106:B106)</f>
         <v>60545</v>
       </c>
       <c r="M106" s="1">
-        <f t="shared" ref="M106:M129" si="2">C106</f>
+        <f t="shared" ref="M106:M129" si="6">C106</f>
         <v>19670</v>
       </c>
       <c r="N106" s="1">
-        <f t="shared" ref="N106:N129" si="3">D106</f>
+        <f t="shared" ref="N106:N129" si="7">D106</f>
         <v>6509</v>
       </c>
       <c r="O106" s="1">
-        <f t="shared" ref="O106:O129" si="4">E106</f>
+        <f t="shared" ref="O106:O129" si="8">E106</f>
         <v>2011</v>
       </c>
       <c r="Q106">
-        <f>(B106+A106)/SUM($A106:$D106)</f>
+        <f t="shared" si="1"/>
         <v>0.69813431114800972</v>
       </c>
       <c r="R106">
-        <f>(C106)/SUM($A106:$E106)</f>
+        <f t="shared" si="2"/>
         <v>0.22167126838338874</v>
       </c>
       <c r="S106">
-        <f>(D106)/SUM($A106:$E106)</f>
+        <f t="shared" si="3"/>
         <v>7.3353242801600271E-2</v>
       </c>
       <c r="T106">
-        <f>(E106)/SUM($A106:$E106)</f>
+        <f t="shared" si="4"/>
         <v>2.2662985293289008E-2</v>
       </c>
     </row>
@@ -2805,35 +3103,35 @@
         <v>1992</v>
       </c>
       <c r="L107">
+        <f t="shared" si="5"/>
+        <v>62386</v>
+      </c>
+      <c r="M107" s="1">
+        <f t="shared" si="6"/>
+        <v>20293</v>
+      </c>
+      <c r="N107" s="1">
+        <f t="shared" si="7"/>
+        <v>6179</v>
+      </c>
+      <c r="O107" s="1">
+        <f t="shared" si="8"/>
+        <v>1114</v>
+      </c>
+      <c r="Q107">
         <f t="shared" si="1"/>
-        <v>62386</v>
-      </c>
-      <c r="M107" s="1">
+        <v>0.70208647505007993</v>
+      </c>
+      <c r="R107">
         <f t="shared" si="2"/>
-        <v>20293</v>
-      </c>
-      <c r="N107" s="1">
+        <v>0.22554794825056684</v>
+      </c>
+      <c r="S107">
         <f t="shared" si="3"/>
-        <v>6179</v>
-      </c>
-      <c r="O107" s="1">
+        <v>6.867692170897613E-2</v>
+      </c>
+      <c r="T107">
         <f t="shared" si="4"/>
-        <v>1114</v>
-      </c>
-      <c r="Q107">
-        <f>(B107+A107)/SUM($A107:$D107)</f>
-        <v>0.70208647505007993</v>
-      </c>
-      <c r="R107">
-        <f>(C107)/SUM($A107:$E107)</f>
-        <v>0.22554794825056684</v>
-      </c>
-      <c r="S107">
-        <f>(D107)/SUM($A107:$E107)</f>
-        <v>6.867692170897613E-2</v>
-      </c>
-      <c r="T107">
-        <f>(E107)/SUM($A107:$E107)</f>
         <v>1.238162984039479E-2</v>
       </c>
     </row>
@@ -2857,35 +3155,35 @@
         <v>1993</v>
       </c>
       <c r="L108">
+        <f t="shared" si="5"/>
+        <v>61314</v>
+      </c>
+      <c r="M108" s="1">
+        <f t="shared" si="6"/>
+        <v>15964</v>
+      </c>
+      <c r="N108" s="1">
+        <f t="shared" si="7"/>
+        <v>7725</v>
+      </c>
+      <c r="O108" s="1">
+        <f t="shared" si="8"/>
+        <v>933</v>
+      </c>
+      <c r="Q108">
         <f t="shared" si="1"/>
-        <v>61314</v>
-      </c>
-      <c r="M108" s="1">
+        <v>0.72131571826876695</v>
+      </c>
+      <c r="R108">
         <f t="shared" si="2"/>
-        <v>15964</v>
-      </c>
-      <c r="N108" s="1">
+        <v>0.18576615155464532</v>
+      </c>
+      <c r="S108">
         <f t="shared" si="3"/>
-        <v>7725</v>
-      </c>
-      <c r="O108" s="1">
+        <v>8.9892478123254516E-2</v>
+      </c>
+      <c r="T108">
         <f t="shared" si="4"/>
-        <v>933</v>
-      </c>
-      <c r="Q108">
-        <f>(B108+A108)/SUM($A108:$D108)</f>
-        <v>0.72131571826876695</v>
-      </c>
-      <c r="R108">
-        <f>(C108)/SUM($A108:$E108)</f>
-        <v>0.18576615155464532</v>
-      </c>
-      <c r="S108">
-        <f>(D108)/SUM($A108:$E108)</f>
-        <v>8.9892478123254516E-2</v>
-      </c>
-      <c r="T108">
-        <f>(E108)/SUM($A108:$E108)</f>
         <v>1.0856916775274623E-2</v>
       </c>
     </row>
@@ -2909,35 +3207,35 @@
         <v>1994</v>
       </c>
       <c r="L109">
+        <f t="shared" si="5"/>
+        <v>57242</v>
+      </c>
+      <c r="M109" s="1">
+        <f t="shared" si="6"/>
+        <v>16952</v>
+      </c>
+      <c r="N109" s="1">
+        <f t="shared" si="7"/>
+        <v>7065</v>
+      </c>
+      <c r="O109" s="1">
+        <f t="shared" si="8"/>
+        <v>928</v>
+      </c>
+      <c r="Q109">
         <f t="shared" si="1"/>
-        <v>57242</v>
-      </c>
-      <c r="M109" s="1">
+        <v>0.70443889292263007</v>
+      </c>
+      <c r="R109">
         <f t="shared" si="2"/>
-        <v>16952</v>
-      </c>
-      <c r="N109" s="1">
+        <v>0.20626133086741213</v>
+      </c>
+      <c r="S109">
         <f t="shared" si="3"/>
-        <v>7065</v>
-      </c>
-      <c r="O109" s="1">
+        <v>8.5962500152092183E-2</v>
+      </c>
+      <c r="T109">
         <f t="shared" si="4"/>
-        <v>928</v>
-      </c>
-      <c r="Q109">
-        <f>(B109+A109)/SUM($A109:$D109)</f>
-        <v>0.70443889292263007</v>
-      </c>
-      <c r="R109">
-        <f>(C109)/SUM($A109:$E109)</f>
-        <v>0.20626133086741213</v>
-      </c>
-      <c r="S109">
-        <f>(D109)/SUM($A109:$E109)</f>
-        <v>8.5962500152092183E-2</v>
-      </c>
-      <c r="T109">
-        <f>(E109)/SUM($A109:$E109)</f>
         <v>1.1291323445313736E-2</v>
       </c>
     </row>
@@ -2964,35 +3262,35 @@
         <v>10</v>
       </c>
       <c r="L110">
+        <f t="shared" si="5"/>
+        <v>44814</v>
+      </c>
+      <c r="M110" s="1">
+        <f t="shared" si="6"/>
+        <v>15932</v>
+      </c>
+      <c r="N110" s="1">
+        <f t="shared" si="7"/>
+        <v>7462</v>
+      </c>
+      <c r="O110" s="1">
+        <f t="shared" si="8"/>
+        <v>542</v>
+      </c>
+      <c r="Q110">
         <f t="shared" si="1"/>
-        <v>44814</v>
-      </c>
-      <c r="M110" s="1">
+        <v>0.65701970443349755</v>
+      </c>
+      <c r="R110">
         <f t="shared" si="2"/>
-        <v>15932</v>
-      </c>
-      <c r="N110" s="1">
+        <v>0.23173818181818182</v>
+      </c>
+      <c r="S110">
         <f t="shared" si="3"/>
-        <v>7462</v>
-      </c>
-      <c r="O110" s="1">
+        <v>0.10853818181818181</v>
+      </c>
+      <c r="T110">
         <f t="shared" si="4"/>
-        <v>542</v>
-      </c>
-      <c r="Q110">
-        <f>(B110+A110)/SUM($A110:$D110)</f>
-        <v>0.65701970443349755</v>
-      </c>
-      <c r="R110">
-        <f>(C110)/SUM($A110:$E110)</f>
-        <v>0.23173818181818182</v>
-      </c>
-      <c r="S110">
-        <f>(D110)/SUM($A110:$E110)</f>
-        <v>0.10853818181818181</v>
-      </c>
-      <c r="T110">
-        <f>(E110)/SUM($A110:$E110)</f>
         <v>7.8836363636363635E-3</v>
       </c>
     </row>
@@ -3031,35 +3329,35 @@
         <v>0</v>
       </c>
       <c r="L111">
+        <f t="shared" si="5"/>
+        <v>48497</v>
+      </c>
+      <c r="M111" s="1">
+        <f t="shared" si="6"/>
+        <v>14464</v>
+      </c>
+      <c r="N111" s="1">
+        <f t="shared" si="7"/>
+        <v>8083</v>
+      </c>
+      <c r="O111" s="1">
+        <f t="shared" si="8"/>
+        <v>543</v>
+      </c>
+      <c r="Q111">
         <f t="shared" si="1"/>
-        <v>48497</v>
-      </c>
-      <c r="M111" s="1">
+        <v>0.68263329767468051</v>
+      </c>
+      <c r="R111">
         <f t="shared" si="2"/>
-        <v>14464</v>
-      </c>
-      <c r="N111" s="1">
+        <v>0.20204785785128584</v>
+      </c>
+      <c r="S111">
         <f t="shared" si="3"/>
-        <v>8083</v>
-      </c>
-      <c r="O111" s="1">
+        <v>0.11291156215513989</v>
+      </c>
+      <c r="T111">
         <f t="shared" si="4"/>
-        <v>543</v>
-      </c>
-      <c r="Q111">
-        <f>(B111+A111)/SUM($A111:$D111)</f>
-        <v>0.68263329767468051</v>
-      </c>
-      <c r="R111">
-        <f>(C111)/SUM($A111:$E111)</f>
-        <v>0.20204785785128584</v>
-      </c>
-      <c r="S111">
-        <f>(D111)/SUM($A111:$E111)</f>
-        <v>0.11291156215513989</v>
-      </c>
-      <c r="T111">
-        <f>(E111)/SUM($A111:$E111)</f>
         <v>7.5851760794557674E-3</v>
       </c>
     </row>
@@ -3089,47 +3387,47 @@
         <v>7.7840999999999996</v>
       </c>
       <c r="I112">
-        <f>(A112+B112)/(q*$H112)</f>
+        <f t="shared" ref="I112:I129" si="9">(A112+B112)/(q*$H112)</f>
         <v>0.19968435785120159</v>
       </c>
       <c r="J112">
-        <f>C112/(q*$H112)</f>
+        <f t="shared" ref="J112:J129" si="10">C112/(q*$H112)</f>
         <v>4.0488787102264077E-2</v>
       </c>
       <c r="K112">
-        <f>D112/(q*$H112)</f>
+        <f t="shared" ref="K112:K129" si="11">D112/(q*$H112)</f>
         <v>2.7041464041880656E-2</v>
       </c>
       <c r="L112">
+        <f t="shared" si="5"/>
+        <v>66644</v>
+      </c>
+      <c r="M112" s="1">
+        <f t="shared" si="6"/>
+        <v>13513</v>
+      </c>
+      <c r="N112" s="1">
+        <f t="shared" si="7"/>
+        <v>9025</v>
+      </c>
+      <c r="O112" s="1">
+        <f t="shared" si="8"/>
+        <v>543</v>
+      </c>
+      <c r="Q112">
         <f t="shared" si="1"/>
-        <v>66644</v>
-      </c>
-      <c r="M112" s="1">
+        <v>0.74728084142539974</v>
+      </c>
+      <c r="R112">
         <f t="shared" si="2"/>
-        <v>13513</v>
-      </c>
-      <c r="N112" s="1">
+        <v>0.1506046252438005</v>
+      </c>
+      <c r="S112">
         <f t="shared" si="3"/>
-        <v>9025</v>
-      </c>
-      <c r="O112" s="1">
+        <v>0.10058512120367791</v>
+      </c>
+      <c r="T112">
         <f t="shared" si="4"/>
-        <v>543</v>
-      </c>
-      <c r="Q112">
-        <f>(B112+A112)/SUM($A112:$D112)</f>
-        <v>0.74728084142539974</v>
-      </c>
-      <c r="R112">
-        <f>(C112)/SUM($A112:$E112)</f>
-        <v>0.1506046252438005</v>
-      </c>
-      <c r="S112">
-        <f>(D112)/SUM($A112:$E112)</f>
-        <v>0.10058512120367791</v>
-      </c>
-      <c r="T112">
-        <f>(E112)/SUM($A112:$E112)</f>
         <v>6.0518250208971862E-3</v>
       </c>
     </row>
@@ -3159,47 +3457,47 @@
         <v>6.9726999999999997</v>
       </c>
       <c r="I113">
-        <f>(A113+B113)/(q*$H113)</f>
+        <f t="shared" si="9"/>
         <v>0.23907738919887081</v>
       </c>
       <c r="J113">
-        <f>C113/(q*$H113)</f>
+        <f t="shared" si="10"/>
         <v>4.4012931794481097E-2</v>
       </c>
       <c r="K113">
-        <f>D113/(q*$H113)</f>
+        <f t="shared" si="11"/>
         <v>2.8719792703101894E-2</v>
       </c>
       <c r="L113">
+        <f t="shared" si="5"/>
+        <v>71474</v>
+      </c>
+      <c r="M113" s="1">
+        <f t="shared" si="6"/>
+        <v>13158</v>
+      </c>
+      <c r="N113" s="1">
+        <f t="shared" si="7"/>
+        <v>8586</v>
+      </c>
+      <c r="O113" s="1">
+        <f t="shared" si="8"/>
+        <v>740</v>
+      </c>
+      <c r="Q113">
         <f t="shared" si="1"/>
-        <v>71474</v>
-      </c>
-      <c r="M113" s="1">
+        <v>0.76674032912098522</v>
+      </c>
+      <c r="R113">
         <f t="shared" si="2"/>
-        <v>13158</v>
-      </c>
-      <c r="N113" s="1">
+        <v>0.140041295046723</v>
+      </c>
+      <c r="S113">
         <f t="shared" si="3"/>
-        <v>8586</v>
-      </c>
-      <c r="O113" s="1">
+        <v>9.1381255454564811E-2</v>
+      </c>
+      <c r="T113">
         <f t="shared" si="4"/>
-        <v>740</v>
-      </c>
-      <c r="Q113">
-        <f>(B113+A113)/SUM($A113:$D113)</f>
-        <v>0.76674032912098522</v>
-      </c>
-      <c r="R113">
-        <f>(C113)/SUM($A113:$E113)</f>
-        <v>0.140041295046723</v>
-      </c>
-      <c r="S113">
-        <f>(D113)/SUM($A113:$E113)</f>
-        <v>9.1381255454564811E-2</v>
-      </c>
-      <c r="T113">
-        <f>(E113)/SUM($A113:$E113)</f>
         <v>7.875859426552289E-3</v>
       </c>
     </row>
@@ -3233,43 +3531,43 @@
         <v>0.28276646588142235</v>
       </c>
       <c r="J114">
-        <f>C114/(q*$H114)</f>
+        <f t="shared" si="10"/>
         <v>5.0422479578402506E-2</v>
       </c>
       <c r="K114">
-        <f>D114/(q*$H114)</f>
+        <f t="shared" si="11"/>
         <v>2.7471018665758424E-2</v>
       </c>
       <c r="L114">
+        <f t="shared" si="5"/>
+        <v>75954</v>
+      </c>
+      <c r="M114" s="1">
+        <f t="shared" si="6"/>
+        <v>13544</v>
+      </c>
+      <c r="N114" s="1">
+        <f t="shared" si="7"/>
+        <v>7379</v>
+      </c>
+      <c r="O114" s="1">
+        <f t="shared" si="8"/>
+        <v>745</v>
+      </c>
+      <c r="Q114">
         <f t="shared" si="1"/>
-        <v>75954</v>
-      </c>
-      <c r="M114" s="1">
+        <v>0.78402510399785297</v>
+      </c>
+      <c r="R114">
         <f t="shared" si="2"/>
-        <v>13544</v>
-      </c>
-      <c r="N114" s="1">
+        <v>0.13873921861875396</v>
+      </c>
+      <c r="S114">
         <f t="shared" si="3"/>
-        <v>7379</v>
-      </c>
-      <c r="O114" s="1">
+        <v>7.5587470037491555E-2</v>
+      </c>
+      <c r="T114">
         <f t="shared" si="4"/>
-        <v>745</v>
-      </c>
-      <c r="Q114">
-        <f>(B114+A114)/SUM($A114:$D114)</f>
-        <v>0.78402510399785297</v>
-      </c>
-      <c r="R114">
-        <f>(C114)/SUM($A114:$E114)</f>
-        <v>0.13873921861875396</v>
-      </c>
-      <c r="S114">
-        <f>(D114)/SUM($A114:$E114)</f>
-        <v>7.5587470037491555E-2</v>
-      </c>
-      <c r="T114">
-        <f>(E114)/SUM($A114:$E114)</f>
         <v>7.6314765114420926E-3</v>
       </c>
     </row>
@@ -3299,47 +3597,47 @@
         <v>6.6265000000000001</v>
       </c>
       <c r="I115">
-        <f>(A115+B115)/(q*$H115)</f>
+        <f t="shared" si="9"/>
         <v>0.24547531115588125</v>
       </c>
       <c r="J115">
-        <f>C115/(q*$H115)</f>
+        <f t="shared" si="10"/>
         <v>4.5833696598538719E-2</v>
       </c>
       <c r="K115">
-        <f>D115/(q*$H115)</f>
+        <f t="shared" si="11"/>
         <v>3.1709090205516453E-2</v>
       </c>
       <c r="L115">
+        <f t="shared" si="5"/>
+        <v>69743</v>
+      </c>
+      <c r="M115" s="1">
+        <f t="shared" si="6"/>
+        <v>13022</v>
+      </c>
+      <c r="N115" s="1">
+        <f t="shared" si="7"/>
+        <v>9009</v>
+      </c>
+      <c r="O115" s="1">
+        <f t="shared" si="8"/>
+        <v>757</v>
+      </c>
+      <c r="Q115">
         <f t="shared" si="1"/>
-        <v>69743</v>
-      </c>
-      <c r="M115" s="1">
+        <v>0.75994290321877656</v>
+      </c>
+      <c r="R115">
         <f t="shared" si="2"/>
-        <v>13022</v>
-      </c>
-      <c r="N115" s="1">
+        <v>0.14073121440382141</v>
+      </c>
+      <c r="S115">
         <f t="shared" si="3"/>
-        <v>9009</v>
-      </c>
-      <c r="O115" s="1">
+        <v>9.7361965179237231E-2</v>
+      </c>
+      <c r="T115">
         <f t="shared" si="4"/>
-        <v>757</v>
-      </c>
-      <c r="Q115">
-        <f>(B115+A115)/SUM($A115:$D115)</f>
-        <v>0.75994290321877656</v>
-      </c>
-      <c r="R115">
-        <f>(C115)/SUM($A115:$E115)</f>
-        <v>0.14073121440382141</v>
-      </c>
-      <c r="S115">
-        <f>(D115)/SUM($A115:$E115)</f>
-        <v>9.7361965179237231E-2</v>
-      </c>
-      <c r="T115">
-        <f>(E115)/SUM($A115:$E115)</f>
         <v>8.1810420291577955E-3</v>
       </c>
     </row>
@@ -3369,47 +3667,47 @@
         <v>6.3841999999999999</v>
       </c>
       <c r="I116">
-        <f>(A116+B116)/(q*$H116)</f>
+        <f t="shared" si="9"/>
         <v>0.26445116900008186</v>
       </c>
       <c r="J116">
-        <f>C116/(q*$H116)</f>
+        <f t="shared" si="10"/>
         <v>4.7036191593463665E-2</v>
       </c>
       <c r="K116">
-        <f>D116/(q*$H116)</f>
+        <f t="shared" si="11"/>
         <v>2.960631430473239E-2</v>
       </c>
       <c r="L116">
+        <f t="shared" si="5"/>
+        <v>72387</v>
+      </c>
+      <c r="M116" s="1">
+        <f t="shared" si="6"/>
+        <v>12875</v>
+      </c>
+      <c r="N116" s="1">
+        <f t="shared" si="7"/>
+        <v>8104</v>
+      </c>
+      <c r="O116" s="1">
+        <f t="shared" si="8"/>
+        <v>772</v>
+      </c>
+      <c r="Q116">
         <f t="shared" si="1"/>
-        <v>72387</v>
-      </c>
-      <c r="M116" s="1">
+        <v>0.7753036437246964</v>
+      </c>
+      <c r="R116">
         <f t="shared" si="2"/>
-        <v>12875</v>
-      </c>
-      <c r="N116" s="1">
+        <v>0.13676729907157578</v>
+      </c>
+      <c r="S116">
         <f t="shared" si="3"/>
-        <v>8104</v>
-      </c>
-      <c r="O116" s="1">
+        <v>8.6086383819499027E-2</v>
+      </c>
+      <c r="T116">
         <f t="shared" si="4"/>
-        <v>772</v>
-      </c>
-      <c r="Q116">
-        <f>(B116+A116)/SUM($A116:$D116)</f>
-        <v>0.7753036437246964</v>
-      </c>
-      <c r="R116">
-        <f>(C116)/SUM($A116:$E116)</f>
-        <v>0.13676729907157578</v>
-      </c>
-      <c r="S116">
-        <f>(D116)/SUM($A116:$E116)</f>
-        <v>8.6086383819499027E-2</v>
-      </c>
-      <c r="T116">
-        <f>(E116)/SUM($A116:$E116)</f>
         <v>8.2007265928742915E-3</v>
       </c>
     </row>
@@ -3439,47 +3737,47 @@
         <v>6.3893000000000004</v>
       </c>
       <c r="I117">
-        <f>(A117+B117)/(q*$H117)</f>
+        <f t="shared" si="9"/>
         <v>0.27881605025460526</v>
       </c>
       <c r="J117">
-        <f>C117/(q*$H117)</f>
+        <f t="shared" si="10"/>
         <v>4.5005539193362504E-2</v>
       </c>
       <c r="K117">
-        <f>D117/(q*$H117)</f>
+        <f t="shared" si="11"/>
         <v>2.9246847272059402E-2</v>
       </c>
       <c r="L117">
+        <f t="shared" si="5"/>
+        <v>76380</v>
+      </c>
+      <c r="M117" s="1">
+        <f t="shared" si="6"/>
+        <v>12329</v>
+      </c>
+      <c r="N117" s="1">
+        <f t="shared" si="7"/>
+        <v>8012</v>
+      </c>
+      <c r="O117" s="1">
+        <f t="shared" si="8"/>
+        <v>771</v>
+      </c>
+      <c r="Q117">
         <f t="shared" si="1"/>
-        <v>76380</v>
-      </c>
-      <c r="M117" s="1">
+        <v>0.78969406850632229</v>
+      </c>
+      <c r="R117">
         <f t="shared" si="2"/>
-        <v>12329</v>
-      </c>
-      <c r="N117" s="1">
+        <v>0.12646165839248349</v>
+      </c>
+      <c r="S117">
         <f t="shared" si="3"/>
-        <v>8012</v>
-      </c>
-      <c r="O117" s="1">
+        <v>8.2181102039141668E-2</v>
+      </c>
+      <c r="T117">
         <f t="shared" si="4"/>
-        <v>771</v>
-      </c>
-      <c r="Q117">
-        <f>(B117+A117)/SUM($A117:$D117)</f>
-        <v>0.78969406850632229</v>
-      </c>
-      <c r="R117">
-        <f>(C117)/SUM($A117:$E117)</f>
-        <v>0.12646165839248349</v>
-      </c>
-      <c r="S117">
-        <f>(D117)/SUM($A117:$E117)</f>
-        <v>8.2181102039141668E-2</v>
-      </c>
-      <c r="T117">
-        <f>(E117)/SUM($A117:$E117)</f>
         <v>7.9083411972264393E-3</v>
       </c>
     </row>
@@ -3509,47 +3807,47 @@
         <v>5.7876000000000003</v>
       </c>
       <c r="I118">
-        <f>(A118+B118)/(q*$H118)</f>
+        <f t="shared" si="9"/>
         <v>0.30313214426611823</v>
       </c>
       <c r="J118">
-        <f>C118/(q*$H118)</f>
+        <f t="shared" si="10"/>
         <v>4.9599851525868877E-2</v>
       </c>
       <c r="K118">
-        <f>D118/(q*$H118)</f>
+        <f t="shared" si="11"/>
         <v>3.7667355558360122E-2</v>
       </c>
       <c r="L118">
+        <f t="shared" si="5"/>
+        <v>75221</v>
+      </c>
+      <c r="M118" s="1">
+        <f t="shared" si="6"/>
+        <v>12308</v>
+      </c>
+      <c r="N118" s="1">
+        <f t="shared" si="7"/>
+        <v>9347</v>
+      </c>
+      <c r="O118" s="1">
+        <f t="shared" si="8"/>
+        <v>1376</v>
+      </c>
+      <c r="Q118">
         <f t="shared" si="1"/>
-        <v>75221</v>
-      </c>
-      <c r="M118" s="1">
+        <v>0.77646682356827279</v>
+      </c>
+      <c r="R118">
         <f t="shared" si="2"/>
-        <v>12308</v>
-      </c>
-      <c r="N118" s="1">
+        <v>0.1252697146114074</v>
+      </c>
+      <c r="S118">
         <f t="shared" si="3"/>
-        <v>9347</v>
-      </c>
-      <c r="O118" s="1">
+        <v>9.5132923502829453E-2</v>
+      </c>
+      <c r="T118">
         <f t="shared" si="4"/>
-        <v>1376</v>
-      </c>
-      <c r="Q118">
-        <f>(B118+A118)/SUM($A118:$D118)</f>
-        <v>0.77646682356827279</v>
-      </c>
-      <c r="R118">
-        <f>(C118)/SUM($A118:$E118)</f>
-        <v>0.1252697146114074</v>
-      </c>
-      <c r="S118">
-        <f>(D118)/SUM($A118:$E118)</f>
-        <v>9.5132923502829453E-2</v>
-      </c>
-      <c r="T118">
-        <f>(E118)/SUM($A118:$E118)</f>
         <v>1.4004803973456012E-2</v>
       </c>
     </row>
@@ -3579,47 +3877,47 @@
         <v>6.4579000000000004</v>
       </c>
       <c r="I119">
-        <f>(A119+B119)/(q*$H119)</f>
+        <f t="shared" si="9"/>
         <v>0.27236547632330377</v>
       </c>
       <c r="J119">
-        <f>C119/(q*$H119)</f>
+        <f t="shared" si="10"/>
         <v>4.4386608640483244E-2</v>
       </c>
       <c r="K119">
-        <f>D119/(q*$H119)</f>
+        <f t="shared" si="11"/>
         <v>3.865499367608561E-2</v>
       </c>
       <c r="L119">
+        <f t="shared" si="5"/>
+        <v>75414</v>
+      </c>
+      <c r="M119" s="1">
+        <f t="shared" si="6"/>
+        <v>12290</v>
+      </c>
+      <c r="N119" s="1">
+        <f t="shared" si="7"/>
+        <v>10703</v>
+      </c>
+      <c r="O119" s="1">
+        <f t="shared" si="8"/>
+        <v>1548</v>
+      </c>
+      <c r="Q119">
         <f t="shared" si="1"/>
-        <v>75414</v>
-      </c>
-      <c r="M119" s="1">
+        <v>0.76634792240389404</v>
+      </c>
+      <c r="R119">
         <f t="shared" si="2"/>
-        <v>12290</v>
-      </c>
-      <c r="N119" s="1">
+        <v>0.1229553298984543</v>
+      </c>
+      <c r="S119">
         <f t="shared" si="3"/>
-        <v>10703</v>
-      </c>
-      <c r="O119" s="1">
+        <v>0.10707818518333249</v>
+      </c>
+      <c r="T119">
         <f t="shared" si="4"/>
-        <v>1548</v>
-      </c>
-      <c r="Q119">
-        <f>(B119+A119)/SUM($A119:$D119)</f>
-        <v>0.76634792240389404</v>
-      </c>
-      <c r="R119">
-        <f>(C119)/SUM($A119:$E119)</f>
-        <v>0.1229553298984543</v>
-      </c>
-      <c r="S119">
-        <f>(D119)/SUM($A119:$E119)</f>
-        <v>0.10707818518333249</v>
-      </c>
-      <c r="T119">
-        <f>(E119)/SUM($A119:$E119)</f>
         <v>1.548696913611125E-2</v>
       </c>
     </row>
@@ -3649,47 +3947,47 @@
         <v>5.9282000000000004</v>
       </c>
       <c r="I120">
-        <f>(A120+B120)/(q*$H120)</f>
+        <f t="shared" si="9"/>
         <v>0.29128842573042402</v>
       </c>
       <c r="J120">
-        <f>C120/(q*$H120)</f>
+        <f t="shared" si="10"/>
         <v>5.1027997538069636E-2</v>
       </c>
       <c r="K120">
-        <f>D120/(q*$H120)</f>
+        <f t="shared" si="11"/>
         <v>4.2722669642706108E-2</v>
       </c>
       <c r="L120">
+        <f t="shared" si="5"/>
+        <v>74038</v>
+      </c>
+      <c r="M120" s="1">
+        <f t="shared" si="6"/>
+        <v>12970</v>
+      </c>
+      <c r="N120" s="1">
+        <f t="shared" si="7"/>
+        <v>10859</v>
+      </c>
+      <c r="O120" s="1">
+        <f t="shared" si="8"/>
+        <v>1537</v>
+      </c>
+      <c r="Q120">
         <f t="shared" si="1"/>
-        <v>74038</v>
-      </c>
-      <c r="M120" s="1">
+        <v>0.7565164968784166</v>
+      </c>
+      <c r="R120">
         <f t="shared" si="2"/>
-        <v>12970</v>
-      </c>
-      <c r="N120" s="1">
+        <v>0.13047764677477766</v>
+      </c>
+      <c r="S120">
         <f t="shared" si="3"/>
-        <v>10859</v>
-      </c>
-      <c r="O120" s="1">
+        <v>0.10924107681783429</v>
+      </c>
+      <c r="T120">
         <f t="shared" si="4"/>
-        <v>1537</v>
-      </c>
-      <c r="Q120">
-        <f>(B120+A120)/SUM($A120:$D120)</f>
-        <v>0.7565164968784166</v>
-      </c>
-      <c r="R120">
-        <f>(C120)/SUM($A120:$E120)</f>
-        <v>0.13047764677477766</v>
-      </c>
-      <c r="S120">
-        <f>(D120)/SUM($A120:$E120)</f>
-        <v>0.10924107681783429</v>
-      </c>
-      <c r="T120">
-        <f>(E120)/SUM($A120:$E120)</f>
         <v>1.5462154440465172E-2</v>
       </c>
     </row>
@@ -3719,47 +4017,47 @@
         <v>5.4306000000000001</v>
       </c>
       <c r="I121">
-        <f>(A121+B121)/(q*$H121)</f>
+        <f t="shared" si="9"/>
         <v>0.30253904024273381</v>
       </c>
       <c r="J121">
-        <f>C121/(q*$H121)</f>
+        <f t="shared" si="10"/>
         <v>5.4943457005313424E-2</v>
       </c>
       <c r="K121">
-        <f>D121/(q*$H121)</f>
+        <f t="shared" si="11"/>
         <v>4.3768371010798807E-2</v>
       </c>
       <c r="L121">
+        <f t="shared" si="5"/>
+        <v>70443</v>
+      </c>
+      <c r="M121" s="1">
+        <f t="shared" si="6"/>
+        <v>12793</v>
+      </c>
+      <c r="N121" s="1">
+        <f t="shared" si="7"/>
+        <v>10191</v>
+      </c>
+      <c r="O121" s="1">
+        <f t="shared" si="8"/>
+        <v>1481</v>
+      </c>
+      <c r="Q121">
         <f t="shared" si="1"/>
-        <v>70443</v>
-      </c>
-      <c r="M121" s="1">
+        <v>0.75398974600490221</v>
+      </c>
+      <c r="R121">
         <f t="shared" si="2"/>
-        <v>12793</v>
-      </c>
-      <c r="N121" s="1">
+        <v>0.13479369494668522</v>
+      </c>
+      <c r="S121">
         <f t="shared" si="3"/>
-        <v>10191</v>
-      </c>
-      <c r="O121" s="1">
+        <v>0.10737767100771273</v>
+      </c>
+      <c r="T121">
         <f t="shared" si="4"/>
-        <v>1481</v>
-      </c>
-      <c r="Q121">
-        <f>(B121+A121)/SUM($A121:$D121)</f>
-        <v>0.75398974600490221</v>
-      </c>
-      <c r="R121">
-        <f>(C121)/SUM($A121:$E121)</f>
-        <v>0.13479369494668522</v>
-      </c>
-      <c r="S121">
-        <f>(D121)/SUM($A121:$E121)</f>
-        <v>0.10737767100771273</v>
-      </c>
-      <c r="T121">
-        <f>(E121)/SUM($A121:$E121)</f>
         <v>1.5604585493319846E-2</v>
       </c>
     </row>
@@ -3789,47 +4087,47 @@
         <v>5.7267000000000001</v>
       </c>
       <c r="I122">
-        <f>(A122+B122)/(q*$H122)</f>
+        <f t="shared" si="9"/>
         <v>0.26659765841756311</v>
       </c>
       <c r="J122">
-        <f>C122/(q*$H122)</f>
+        <f t="shared" si="10"/>
         <v>4.8828111134728062E-2</v>
       </c>
       <c r="K122">
-        <f>D122/(q*$H122)</f>
+        <f t="shared" si="11"/>
         <v>4.6677703037377456E-2</v>
       </c>
       <c r="L122">
+        <f t="shared" si="5"/>
+        <v>65459</v>
+      </c>
+      <c r="M122" s="1">
+        <f t="shared" si="6"/>
+        <v>11989</v>
+      </c>
+      <c r="N122" s="1">
+        <f t="shared" si="7"/>
+        <v>11461</v>
+      </c>
+      <c r="O122" s="1">
+        <f t="shared" si="8"/>
+        <v>1486</v>
+      </c>
+      <c r="Q122">
         <f t="shared" si="1"/>
-        <v>65459</v>
-      </c>
-      <c r="M122" s="1">
+        <v>0.73624717407686513</v>
+      </c>
+      <c r="R122">
         <f t="shared" si="2"/>
-        <v>11989</v>
-      </c>
-      <c r="N122" s="1">
+        <v>0.13262901709165331</v>
+      </c>
+      <c r="S122">
         <f t="shared" si="3"/>
-        <v>11461</v>
-      </c>
-      <c r="O122" s="1">
+        <v>0.12678798606117594</v>
+      </c>
+      <c r="T122">
         <f t="shared" si="4"/>
-        <v>1486</v>
-      </c>
-      <c r="Q122">
-        <f>(B122+A122)/SUM($A122:$D122)</f>
-        <v>0.73624717407686513</v>
-      </c>
-      <c r="R122">
-        <f>(C122)/SUM($A122:$E122)</f>
-        <v>0.13262901709165331</v>
-      </c>
-      <c r="S122">
-        <f>(D122)/SUM($A122:$E122)</f>
-        <v>0.12678798606117594</v>
-      </c>
-      <c r="T122">
-        <f>(E122)/SUM($A122:$E122)</f>
         <v>1.643896233198739E-2</v>
       </c>
     </row>
@@ -3859,47 +4157,47 @@
         <v>5.6536</v>
       </c>
       <c r="I123">
-        <f>(A123+B123)/(q*$H123)</f>
+        <f t="shared" si="9"/>
         <v>0.25300267934326398</v>
       </c>
       <c r="J123">
-        <f>C123/(q*$H123)</f>
+        <f t="shared" si="10"/>
         <v>4.7862918825667698E-2</v>
       </c>
       <c r="K123">
-        <f>D123/(q*$H123)</f>
+        <f t="shared" si="11"/>
         <v>4.4030419981585189E-2</v>
       </c>
       <c r="L123">
+        <f t="shared" si="5"/>
+        <v>61328</v>
+      </c>
+      <c r="M123" s="1">
+        <f t="shared" si="6"/>
+        <v>11602</v>
+      </c>
+      <c r="N123" s="1">
+        <f t="shared" si="7"/>
+        <v>10673</v>
+      </c>
+      <c r="O123" s="1">
+        <f t="shared" si="8"/>
+        <v>1344</v>
+      </c>
+      <c r="Q123">
         <f t="shared" si="1"/>
-        <v>61328</v>
-      </c>
-      <c r="M123" s="1">
+        <v>0.73356219274427947</v>
+      </c>
+      <c r="R123">
         <f t="shared" si="2"/>
-        <v>11602</v>
-      </c>
-      <c r="N123" s="1">
+        <v>0.13657927884445595</v>
+      </c>
+      <c r="S123">
         <f t="shared" si="3"/>
-        <v>10673</v>
-      </c>
-      <c r="O123" s="1">
+        <v>0.12564304801817605</v>
+      </c>
+      <c r="T123">
         <f t="shared" si="4"/>
-        <v>1344</v>
-      </c>
-      <c r="Q123">
-        <f>(B123+A123)/SUM($A123:$D123)</f>
-        <v>0.73356219274427947</v>
-      </c>
-      <c r="R123">
-        <f>(C123)/SUM($A123:$E123)</f>
-        <v>0.13657927884445595</v>
-      </c>
-      <c r="S123">
-        <f>(D123)/SUM($A123:$E123)</f>
-        <v>0.12564304801817605</v>
-      </c>
-      <c r="T123">
-        <f>(E123)/SUM($A123:$E123)</f>
         <v>1.5821629957502914E-2</v>
       </c>
     </row>
@@ -3929,47 +4227,47 @@
         <v>5.4951999999999996</v>
       </c>
       <c r="I124">
-        <f>(A124+B124)/(q*$H124)</f>
+        <f t="shared" si="9"/>
         <v>0.23339079072583607</v>
       </c>
       <c r="J124">
-        <f>C124/(q*$H124)</f>
+        <f t="shared" si="10"/>
         <v>4.7039774020521216E-2</v>
       </c>
       <c r="K124">
-        <f>D124/(q*$H124)</f>
+        <f t="shared" si="11"/>
         <v>3.727784311307749E-2</v>
       </c>
       <c r="L124">
+        <f t="shared" si="5"/>
+        <v>54989</v>
+      </c>
+      <c r="M124" s="1">
+        <f t="shared" si="6"/>
+        <v>11083</v>
+      </c>
+      <c r="N124" s="1">
+        <f t="shared" si="7"/>
+        <v>8783</v>
+      </c>
+      <c r="O124" s="1">
+        <f t="shared" si="8"/>
+        <v>1308</v>
+      </c>
+      <c r="Q124">
         <f t="shared" si="1"/>
-        <v>54989</v>
-      </c>
-      <c r="M124" s="1">
+        <v>0.73460690668626005</v>
+      </c>
+      <c r="R124">
         <f t="shared" si="2"/>
-        <v>11083</v>
-      </c>
-      <c r="N124" s="1">
+        <v>0.14551685201475781</v>
+      </c>
+      <c r="S124">
         <f t="shared" si="3"/>
-        <v>8783</v>
-      </c>
-      <c r="O124" s="1">
+        <v>0.11531846172025786</v>
+      </c>
+      <c r="T124">
         <f t="shared" si="4"/>
-        <v>1308</v>
-      </c>
-      <c r="Q124">
-        <f>(B124+A124)/SUM($A124:$D124)</f>
-        <v>0.73460690668626005</v>
-      </c>
-      <c r="R124">
-        <f>(C124)/SUM($A124:$E124)</f>
-        <v>0.14551685201475781</v>
-      </c>
-      <c r="S124">
-        <f>(D124)/SUM($A124:$E124)</f>
-        <v>0.11531846172025786</v>
-      </c>
-      <c r="T124">
-        <f>(E124)/SUM($A124:$E124)</f>
         <v>1.7173693263133016E-2</v>
       </c>
     </row>
@@ -3999,47 +4297,47 @@
         <v>5.1238999999999999</v>
       </c>
       <c r="I125">
-        <f>(A125+B125)/(q*$H125)</f>
+        <f t="shared" si="9"/>
         <v>0.24091732347373335</v>
       </c>
       <c r="J125">
-        <f>C125/(q*$H125)</f>
+        <f t="shared" si="10"/>
         <v>4.7102848514107974E-2</v>
       </c>
       <c r="K125">
-        <f>D125/(q*$H125)</f>
+        <f t="shared" si="11"/>
         <v>3.5718598017994325E-2</v>
       </c>
       <c r="L125">
+        <f t="shared" si="5"/>
+        <v>52927</v>
+      </c>
+      <c r="M125" s="1">
+        <f t="shared" si="6"/>
+        <v>10348</v>
+      </c>
+      <c r="N125" s="1">
+        <f t="shared" si="7"/>
+        <v>7847</v>
+      </c>
+      <c r="O125" s="1">
+        <f t="shared" si="8"/>
+        <v>1239</v>
+      </c>
+      <c r="Q125">
         <f t="shared" si="1"/>
-        <v>52927</v>
-      </c>
-      <c r="M125" s="1">
+        <v>0.74417198616461855</v>
+      </c>
+      <c r="R125">
         <f t="shared" si="2"/>
-        <v>10348</v>
-      </c>
-      <c r="N125" s="1">
+        <v>0.14300520998880611</v>
+      </c>
+      <c r="S125">
         <f t="shared" si="3"/>
-        <v>7847</v>
-      </c>
-      <c r="O125" s="1">
+        <v>0.10844239300175509</v>
+      </c>
+      <c r="T125">
         <f t="shared" si="4"/>
-        <v>1239</v>
-      </c>
-      <c r="Q125">
-        <f>(B125+A125)/SUM($A125:$D125)</f>
-        <v>0.74417198616461855</v>
-      </c>
-      <c r="R125">
-        <f>(C125)/SUM($A125:$E125)</f>
-        <v>0.14300520998880611</v>
-      </c>
-      <c r="S125">
-        <f>(D125)/SUM($A125:$E125)</f>
-        <v>0.10844239300175509</v>
-      </c>
-      <c r="T125">
-        <f>(E125)/SUM($A125:$E125)</f>
         <v>1.7122483105540279E-2</v>
       </c>
     </row>
@@ -4069,47 +4367,47 @@
         <v>5.0434999999999999</v>
       </c>
       <c r="I126">
-        <f>(A126+B126)/(q*$H126)</f>
+        <f t="shared" si="9"/>
         <v>0.19410634406901456</v>
       </c>
       <c r="J126">
-        <f>C126/(q*$H126)</f>
+        <f t="shared" si="10"/>
         <v>4.3543749362792226E-2</v>
       </c>
       <c r="K126">
-        <f>D126/(q*$H126)</f>
+        <f t="shared" si="11"/>
         <v>3.2847414159294097E-2</v>
       </c>
       <c r="L126">
+        <f t="shared" si="5"/>
+        <v>41974</v>
+      </c>
+      <c r="M126" s="1">
+        <f t="shared" si="6"/>
+        <v>9416</v>
+      </c>
+      <c r="N126" s="1">
+        <f t="shared" si="7"/>
+        <v>7103</v>
+      </c>
+      <c r="O126" s="1">
+        <f t="shared" si="8"/>
+        <v>1144</v>
+      </c>
+      <c r="Q126">
         <f t="shared" si="1"/>
-        <v>41974</v>
-      </c>
-      <c r="M126" s="1">
+        <v>0.71759013899099033</v>
+      </c>
+      <c r="R126">
         <f t="shared" si="2"/>
-        <v>9416</v>
-      </c>
-      <c r="N126" s="1">
+        <v>0.15788855911598504</v>
+      </c>
+      <c r="S126">
         <f t="shared" si="3"/>
-        <v>7103</v>
-      </c>
-      <c r="O126" s="1">
+        <v>0.11910391200093902</v>
+      </c>
+      <c r="T126">
         <f t="shared" si="4"/>
-        <v>1144</v>
-      </c>
-      <c r="Q126">
-        <f>(B126+A126)/SUM($A126:$D126)</f>
-        <v>0.71759013899099033</v>
-      </c>
-      <c r="R126">
-        <f>(C126)/SUM($A126:$E126)</f>
-        <v>0.15788855911598504</v>
-      </c>
-      <c r="S126">
-        <f>(D126)/SUM($A126:$E126)</f>
-        <v>0.11910391200093902</v>
-      </c>
-      <c r="T126">
-        <f>(E126)/SUM($A126:$E126)</f>
         <v>1.9182722135586968E-2</v>
       </c>
     </row>
@@ -4139,47 +4437,47 @@
         <v>5.5606</v>
       </c>
       <c r="I127">
-        <f>(A127+B127)/(q*$H127)</f>
+        <f t="shared" si="9"/>
         <v>0.14115830405116331</v>
       </c>
       <c r="J127">
-        <f>C127/(q*$H127)</f>
+        <f t="shared" si="10"/>
         <v>4.2376013128570242E-2</v>
       </c>
       <c r="K127">
-        <f>D127/(q*$H127)</f>
+        <f t="shared" si="11"/>
         <v>2.8404470049161409E-2</v>
       </c>
       <c r="L127">
+        <f t="shared" si="5"/>
+        <v>33654</v>
+      </c>
+      <c r="M127" s="1">
+        <f t="shared" si="6"/>
+        <v>10103</v>
+      </c>
+      <c r="N127" s="1">
+        <f t="shared" si="7"/>
+        <v>6772</v>
+      </c>
+      <c r="O127" s="1">
+        <f t="shared" si="8"/>
+        <v>1140</v>
+      </c>
+      <c r="Q127">
         <f t="shared" si="1"/>
-        <v>33654</v>
-      </c>
-      <c r="M127" s="1">
+        <v>0.66603336697737936</v>
+      </c>
+      <c r="R127">
         <f t="shared" si="2"/>
-        <v>10103</v>
-      </c>
-      <c r="N127" s="1">
+        <v>0.19553310495655035</v>
+      </c>
+      <c r="S127">
         <f t="shared" si="3"/>
-        <v>6772</v>
-      </c>
-      <c r="O127" s="1">
+        <v>0.13106504867522112</v>
+      </c>
+      <c r="T127">
         <f t="shared" si="4"/>
-        <v>1140</v>
-      </c>
-      <c r="Q127">
-        <f>(B127+A127)/SUM($A127:$D127)</f>
-        <v>0.66603336697737936</v>
-      </c>
-      <c r="R127">
-        <f>(C127)/SUM($A127:$E127)</f>
-        <v>0.19553310495655035</v>
-      </c>
-      <c r="S127">
-        <f>(D127)/SUM($A127:$E127)</f>
-        <v>0.13106504867522112</v>
-      </c>
-      <c r="T127">
-        <f>(E127)/SUM($A127:$E127)</f>
         <v>2.2063519712013004E-2</v>
       </c>
     </row>
@@ -4209,47 +4507,47 @@
         <v>4.7301000000000002</v>
       </c>
       <c r="I128">
-        <f>(A128+B128)/(q*$H128)</f>
+        <f t="shared" si="9"/>
         <v>0.15025261325319922</v>
       </c>
       <c r="J128">
-        <f>C128/(q*$H128)</f>
+        <f t="shared" si="10"/>
         <v>4.3593572911903855E-2</v>
       </c>
       <c r="K128">
-        <f>D128/(q*$H128)</f>
+        <f t="shared" si="11"/>
         <v>3.7415228057405998E-2</v>
       </c>
       <c r="L128">
+        <f t="shared" si="5"/>
+        <v>30472</v>
+      </c>
+      <c r="M128" s="1">
+        <f t="shared" si="6"/>
+        <v>8841</v>
+      </c>
+      <c r="N128" s="1">
+        <f t="shared" si="7"/>
+        <v>7588</v>
+      </c>
+      <c r="O128" s="1">
+        <f t="shared" si="8"/>
+        <v>1137</v>
+      </c>
+      <c r="Q128">
         <f t="shared" si="1"/>
-        <v>30472</v>
-      </c>
-      <c r="M128" s="1">
+        <v>0.64970896142939383</v>
+      </c>
+      <c r="R128">
         <f t="shared" si="2"/>
-        <v>8841</v>
-      </c>
-      <c r="N128" s="1">
+        <v>0.18404180024147551</v>
+      </c>
+      <c r="S128">
         <f t="shared" si="3"/>
-        <v>7588</v>
-      </c>
-      <c r="O128" s="1">
+        <v>0.15795828302593781</v>
+      </c>
+      <c r="T128">
         <f t="shared" si="4"/>
-        <v>1137</v>
-      </c>
-      <c r="Q128">
-        <f>(B128+A128)/SUM($A128:$D128)</f>
-        <v>0.64970896142939383</v>
-      </c>
-      <c r="R128">
-        <f>(C128)/SUM($A128:$E128)</f>
-        <v>0.18404180024147551</v>
-      </c>
-      <c r="S128">
-        <f>(D128)/SUM($A128:$E128)</f>
-        <v>0.15795828302593781</v>
-      </c>
-      <c r="T128">
-        <f>(E128)/SUM($A128:$E128)</f>
         <v>2.3668762229901327E-2</v>
       </c>
     </row>
@@ -4279,47 +4577,47 @@
         <v>5.1645000000000003</v>
       </c>
       <c r="I129">
-        <f>(A129+B129)/(q*$H129)</f>
+        <f t="shared" si="9"/>
         <v>0.11279851675712529</v>
       </c>
       <c r="J129">
-        <f>C129/(q*$H129)</f>
+        <f t="shared" si="10"/>
         <v>4.2067429378733319E-2</v>
       </c>
       <c r="K129">
-        <f>D129/(q*$H129)</f>
+        <f t="shared" si="11"/>
         <v>3.1987504271558574E-2</v>
       </c>
       <c r="L129">
+        <f t="shared" si="5"/>
+        <v>24977</v>
+      </c>
+      <c r="M129" s="1">
+        <f t="shared" si="6"/>
+        <v>9315</v>
+      </c>
+      <c r="N129" s="1">
+        <f t="shared" si="7"/>
+        <v>7083</v>
+      </c>
+      <c r="O129" s="1">
+        <f t="shared" si="8"/>
+        <v>1137</v>
+      </c>
+      <c r="Q129">
         <f t="shared" si="1"/>
-        <v>24977</v>
-      </c>
-      <c r="M129" s="1">
+        <v>0.60367371601208464</v>
+      </c>
+      <c r="R129">
         <f t="shared" si="2"/>
-        <v>9315</v>
-      </c>
-      <c r="N129" s="1">
+        <v>0.21911460293564169</v>
+      </c>
+      <c r="S129">
         <f t="shared" si="3"/>
-        <v>7083</v>
-      </c>
-      <c r="O129" s="1">
+        <v>0.16661178020323672</v>
+      </c>
+      <c r="T129">
         <f t="shared" si="4"/>
-        <v>1137</v>
-      </c>
-      <c r="Q129">
-        <f>(B129+A129)/SUM($A129:$D129)</f>
-        <v>0.60367371601208464</v>
-      </c>
-      <c r="R129">
-        <f>(C129)/SUM($A129:$E129)</f>
-        <v>0.21911460293564169</v>
-      </c>
-      <c r="S129">
-        <f>(D129)/SUM($A129:$E129)</f>
-        <v>0.16661178020323672</v>
-      </c>
-      <c r="T129">
-        <f>(E129)/SUM($A129:$E129)</f>
         <v>2.6745389537071885E-2</v>
       </c>
     </row>
@@ -4365,31 +4663,34 @@
         <v>59730.239999999998</v>
       </c>
       <c r="M131" s="2">
-        <f t="shared" ref="M131:O131" si="5">AVERAGE(M105:M129)</f>
+        <f t="shared" ref="M131:O131" si="12">AVERAGE(M105:M129)</f>
         <v>13298.24</v>
       </c>
       <c r="N131" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>8285.36</v>
       </c>
       <c r="O131" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>1051.04</v>
+      </c>
+      <c r="P131" t="s">
+        <v>15</v>
       </c>
       <c r="Q131" s="3">
         <f>AVERAGE(Q105:Q129)</f>
         <v>0.7265545875735071</v>
       </c>
       <c r="R131" s="3">
-        <f t="shared" ref="R131:T131" si="6">AVERAGE(R105:R129)</f>
+        <f t="shared" ref="R131:T131" si="13">AVERAGE(R105:R129)</f>
         <v>0.1653820003221641</v>
       </c>
       <c r="S131" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>0.10422311354687325</v>
       </c>
       <c r="T131" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>1.3491464555664136E-2</v>
       </c>
     </row>
@@ -4399,16 +4700,35 @@
         <v>0.58752822732404963</v>
       </c>
       <c r="C132">
-        <f t="shared" ref="C132:E132" si="7">C131/SUM($B$131:$E$131)</f>
+        <f t="shared" ref="C132:E132" si="14">C131/SUM($B$131:$E$131)</f>
         <v>0.21911460293564169</v>
       </c>
       <c r="D132">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>0.16661178020323672</v>
       </c>
       <c r="E132">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>2.6745389537071885E-2</v>
+      </c>
+      <c r="P132" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q132">
+        <f>AVERAGE(Q125:Q129)</f>
+        <v>0.67623563391489339</v>
+      </c>
+      <c r="R132">
+        <f t="shared" ref="R132:T132" si="15">AVERAGE(R125:R129)</f>
+        <v>0.17991665544769173</v>
+      </c>
+      <c r="S132">
+        <f t="shared" si="15"/>
+        <v>0.13663628338141795</v>
+      </c>
+      <c r="T132">
+        <f t="shared" si="15"/>
+        <v>2.1756575344022692E-2</v>
       </c>
     </row>
     <row r="133" spans="1:20">
@@ -4418,6 +4738,22 @@
       <c r="O133" t="s">
         <v>14</v>
       </c>
+      <c r="Q133" s="4">
+        <f>Q132/SUM($Q$132:$T$132)</f>
+        <v>0.66654070071627858</v>
+      </c>
+      <c r="R133" s="4">
+        <f t="shared" ref="R133:T133" si="16">R132/SUM($Q$132:$T$132)</f>
+        <v>0.17733725875753875</v>
+      </c>
+      <c r="S133" s="4">
+        <f t="shared" si="16"/>
+        <v>0.13467738093165948</v>
+      </c>
+      <c r="T133" s="4">
+        <f t="shared" si="16"/>
+        <v>2.144465959452305E-2</v>
+      </c>
     </row>
     <row r="134" spans="1:20">
       <c r="L134" t="s">
@@ -4478,6 +4814,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Fixed bug in TMA2.R
</commit_message>
<xml_diff>
--- a/src/dashboard/data/harvestPolicy/DataFromIan/Removals.xlsx
+++ b/src/dashboard/data/harvestPolicy/DataFromIan/Removals.xlsx
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="q">Sheet1!$H$131</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterate="1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -134,8 +134,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="83">
+  <cellStyleXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -226,7 +252,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="83">
+  <cellStyles count="109">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -268,6 +294,19 @@
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -309,6 +348,19 @@
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -335,10 +387,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -350,11 +398,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$111</c:f>
+              <c:f>Sheet1!$I$111</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>48497</c:v>
+                  <c:v>Commercial</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -424,63 +472,63 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$112:$L$129</c:f>
+              <c:f>Sheet1!$I$112:$I$129</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>66644.0</c:v>
+                  <c:v>0.199684357851202</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>71474.0</c:v>
+                  <c:v>0.239077389198871</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75954.0</c:v>
+                  <c:v>0.282766465881422</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>69743.0</c:v>
+                  <c:v>0.245475311155881</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>72387.0</c:v>
+                  <c:v>0.264451169000082</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>76380.0</c:v>
+                  <c:v>0.278816050254605</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>75221.0</c:v>
+                  <c:v>0.303132144266118</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>75414.0</c:v>
+                  <c:v>0.272365476323304</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>74038.0</c:v>
+                  <c:v>0.291288425730424</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>70443.0</c:v>
+                  <c:v>0.302539040242734</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>65459.0</c:v>
+                  <c:v>0.266597658417563</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>61328.0</c:v>
+                  <c:v>0.253002679343264</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>54989.0</c:v>
+                  <c:v>0.233390790725836</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>52927.0</c:v>
+                  <c:v>0.240917323473733</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>41974.0</c:v>
+                  <c:v>0.194106344069015</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>33654.0</c:v>
+                  <c:v>0.141158304051163</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>30472.0</c:v>
+                  <c:v>0.150252613253199</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>24977.0</c:v>
+                  <c:v>0.112798516757125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -497,6 +545,304 @@
         </c:dLbls>
         <c:axId val="2139200936"/>
         <c:axId val="2139237176"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$111</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bycatch</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$112:$H$129</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>7.784099999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9727</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2649</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.6265</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.3842</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3893</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.7876</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.4579</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.9282</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.4306</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.7267</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.6536</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.4952</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.1239</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.0435</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.5606</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.7301</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.1645</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$112:$J$129</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0.0404887871022641</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0440129317944811</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0504224795784025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0458336965985387</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0470361915934637</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0450055391933625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0495998515258689</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0443866086404832</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0510279975380696</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0549434570053134</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0488281111347281</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0478629188256677</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0470397740205212</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.047102848514108</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0435437493627922</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0423760131285702</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0435935729119038</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0420674293787333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$111</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sport</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$112:$H$129</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>7.784099999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9727</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2649</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.6265</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.3842</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3893</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.7876</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.4579</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.9282</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.4306</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.7267</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.6536</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.4952</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.1239</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.0435</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.5606</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.7301</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.1645</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$112:$K$129</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0.0270414640418807</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0287197927031019</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0274710186657584</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0317090902055164</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0296063143047324</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0292468472720594</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0376673555583601</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0386549936760856</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0427226696427061</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0437683710107988</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0466777030373774</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0440304199815852</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0372778431130775</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0357185980179943</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0328474141592941</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0284044700491614</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.037415228057406</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0319875042715586</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2137782968"/>
+        <c:axId val="2137773224"/>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="2139200936"/>
@@ -529,6 +875,35 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="2137773224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2137782968"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2137782968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2137773224"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -557,8 +932,8 @@
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
       <xdr:row>147</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
@@ -872,7 +1247,7 @@
   <dimension ref="A1:T137"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="I140" sqref="I140"/>
+      <selection activeCell="I112" sqref="I112:I129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>